<commit_message>
add 行政部會 column, correct parsed result
</commit_message>
<xml_diff>
--- a/1_政策宣傳執情形/parsed/農委會/農委會主管101年廣宣彙整.xlsx
+++ b/1_政策宣傳執情形/parsed/農委會/農委會主管101年廣宣彙整.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="405">
   <si>
     <t xml:space="preserve"> 國產牛肉追溯資訊網</t>
   </si>
@@ -1034,6 +1034,9 @@
   </si>
   <si>
     <t>落實海洋保護區管理，兼顧海洋生態保育與海洋資源永續利用</t>
+  </si>
+  <si>
+    <t>行政部會</t>
   </si>
   <si>
     <t>行政院公共工程委員會第12屆公共工程金質獎（水保優良工程事蹟）</t>
@@ -1608,11 +1611,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryRight="1" summaryBelow="1"/>
   </sheetPr>
-  <dimension ref="A1:F233"/>
+  <dimension ref="A1:G233"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1" activeCell="A1"/>
@@ -1620,15 +1623,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col max="1" width="9.10" min="1"/>
-    <col max="2" width="9.10" min="2"/>
-    <col max="3" width="9.10" min="3"/>
-    <col max="4" width="9.10" min="4"/>
-    <col max="5" width="9.10" min="5"/>
-    <col max="6" width="9.10" min="6"/>
+    <col max="1" min="1" width="9.10"/>
+    <col max="2" min="2" width="9.10"/>
+    <col max="3" min="3" width="9.10"/>
+    <col max="4" min="4" width="9.10"/>
+    <col max="5" min="5" width="9.10"/>
+    <col max="6" min="6" width="9.10"/>
+    <col max="7" min="7" width="9.10"/>
   </cols>
   <sheetData>
-    <row spans="1:6" r="1">
+    <row spans="1:7" r="1">
       <c t="s" s="1" r="A1">
         <v>120</v>
       </c>
@@ -1639,18 +1643,21 @@
         <v>257</v>
       </c>
       <c t="s" s="1" r="D1">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c t="s" s="1" r="E1">
         <v>149</v>
       </c>
       <c t="s" s="1" r="F1">
+        <v>333</v>
+      </c>
+      <c t="s" s="1" r="G1">
         <v>123</v>
       </c>
     </row>
-    <row spans="1:6" r="2">
+    <row spans="1:7" r="2">
       <c t="s" r="A2">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c t="s" r="B2">
         <v>151</v>
@@ -1662,10 +1669,13 @@
         <v>335000.0</v>
       </c>
       <c t="s" r="E2">
-        <v>349</v>
-      </c>
-    </row>
-    <row spans="1:6" r="3">
+        <v>350</v>
+      </c>
+      <c t="s" r="F2">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="3">
       <c t="s" r="A3">
         <v>321</v>
       </c>
@@ -1679,10 +1689,13 @@
         <v>0.0</v>
       </c>
       <c t="s" r="E3">
-        <v>349</v>
-      </c>
-    </row>
-    <row spans="1:6" r="4">
+        <v>350</v>
+      </c>
+      <c t="s" r="F3">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="4">
       <c t="s" r="A4">
         <v>322</v>
       </c>
@@ -1696,12 +1709,15 @@
         <v>0.0</v>
       </c>
       <c t="s" r="E4">
-        <v>349</v>
-      </c>
-    </row>
-    <row spans="1:6" r="5">
+        <v>350</v>
+      </c>
+      <c t="s" r="F4">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="5">
       <c t="s" r="A5">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c t="s" r="B5">
         <v>326</v>
@@ -1713,12 +1729,15 @@
         <v>50000.0</v>
       </c>
       <c t="s" r="E5">
-        <v>349</v>
-      </c>
-    </row>
-    <row spans="1:6" r="6">
+        <v>350</v>
+      </c>
+      <c t="s" r="F5">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="6">
       <c t="s" r="A6">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c t="s" r="B6">
         <v>150</v>
@@ -1730,10 +1749,13 @@
         <v>160000.0</v>
       </c>
       <c t="s" r="E6">
-        <v>349</v>
-      </c>
-    </row>
-    <row spans="1:6" r="7">
+        <v>350</v>
+      </c>
+      <c t="s" r="F6">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="7">
       <c t="s" r="A7">
         <v>129</v>
       </c>
@@ -1747,10 +1769,13 @@
         <v>287000.0</v>
       </c>
       <c t="s" r="E7">
-        <v>349</v>
-      </c>
-    </row>
-    <row spans="1:6" r="8">
+        <v>350</v>
+      </c>
+      <c t="s" r="F7">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="8">
       <c t="s" r="A8">
         <v>144</v>
       </c>
@@ -1764,10 +1789,13 @@
         <v>269000.0</v>
       </c>
       <c t="s" r="E8">
-        <v>349</v>
-      </c>
-    </row>
-    <row spans="1:6" r="9">
+        <v>350</v>
+      </c>
+      <c t="s" r="F8">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="9">
       <c t="s" r="A9">
         <v>47</v>
       </c>
@@ -1781,10 +1809,13 @@
         <v>73000.0</v>
       </c>
       <c t="s" r="E9">
-        <v>349</v>
-      </c>
-    </row>
-    <row spans="1:6" r="10">
+        <v>350</v>
+      </c>
+      <c t="s" r="F9">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="10">
       <c t="s" r="A10">
         <v>139</v>
       </c>
@@ -1798,10 +1829,13 @@
         <v>25000.0</v>
       </c>
       <c t="s" r="E10">
-        <v>349</v>
-      </c>
-    </row>
-    <row spans="1:6" r="11">
+        <v>350</v>
+      </c>
+      <c t="s" r="F10">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="11">
       <c t="s" r="A11">
         <v>45</v>
       </c>
@@ -1815,10 +1849,13 @@
         <v>185000.0</v>
       </c>
       <c t="s" r="E11">
-        <v>349</v>
-      </c>
-    </row>
-    <row spans="1:6" r="12">
+        <v>350</v>
+      </c>
+      <c t="s" r="F11">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="12">
       <c t="s" r="A12">
         <v>48</v>
       </c>
@@ -1832,10 +1869,13 @@
         <v>73000.0</v>
       </c>
       <c t="s" r="E12">
-        <v>349</v>
-      </c>
-    </row>
-    <row spans="1:6" r="13">
+        <v>350</v>
+      </c>
+      <c t="s" r="F12">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="13">
       <c t="s" r="A13">
         <v>134</v>
       </c>
@@ -1849,10 +1889,13 @@
         <v>1764743.0</v>
       </c>
       <c t="s" r="E13">
-        <v>349</v>
-      </c>
-    </row>
-    <row spans="1:6" r="14">
+        <v>350</v>
+      </c>
+      <c t="s" r="F13">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="14">
       <c t="s" r="A14">
         <v>145</v>
       </c>
@@ -1866,10 +1909,13 @@
         <v>879306.0</v>
       </c>
       <c t="s" r="E14">
-        <v>349</v>
-      </c>
-    </row>
-    <row spans="1:6" r="15">
+        <v>350</v>
+      </c>
+      <c t="s" r="F14">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="15">
       <c t="s" r="A15">
         <v>7</v>
       </c>
@@ -1883,10 +1929,13 @@
         <v>0.0</v>
       </c>
       <c t="s" r="E15">
-        <v>349</v>
-      </c>
-    </row>
-    <row spans="1:6" r="16">
+        <v>350</v>
+      </c>
+      <c t="s" r="F15">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="16">
       <c t="s" r="A16">
         <v>146</v>
       </c>
@@ -1900,12 +1949,15 @@
         <v>140386.0</v>
       </c>
       <c t="s" r="E16">
-        <v>349</v>
-      </c>
-    </row>
-    <row spans="1:6" r="17">
+        <v>350</v>
+      </c>
+      <c t="s" r="F16">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="17">
       <c t="s" r="A17">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c t="s" r="B17">
         <v>205</v>
@@ -1917,10 +1969,13 @@
         <v>0.0</v>
       </c>
       <c t="s" r="E17">
-        <v>349</v>
-      </c>
-    </row>
-    <row spans="1:6" r="18">
+        <v>350</v>
+      </c>
+      <c t="s" r="F17">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="18">
       <c t="s" r="A18">
         <v>255</v>
       </c>
@@ -1934,10 +1989,13 @@
         <v>0.0</v>
       </c>
       <c t="s" r="E18">
-        <v>349</v>
-      </c>
-    </row>
-    <row spans="1:6" r="19">
+        <v>350</v>
+      </c>
+      <c t="s" r="F18">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="19">
       <c t="s" r="A19">
         <v>255</v>
       </c>
@@ -1951,12 +2009,15 @@
         <v>640200.0</v>
       </c>
       <c t="s" r="E19">
-        <v>349</v>
-      </c>
-    </row>
-    <row spans="1:6" r="20">
+        <v>350</v>
+      </c>
+      <c t="s" r="F19">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="20">
       <c t="s" r="A20">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c t="s" r="B20">
         <v>316</v>
@@ -1968,10 +2029,13 @@
         <v>355990.0</v>
       </c>
       <c t="s" r="E20">
-        <v>349</v>
-      </c>
-    </row>
-    <row spans="1:6" r="21">
+        <v>350</v>
+      </c>
+      <c t="s" r="F20">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="21">
       <c t="s" r="A21">
         <v>218</v>
       </c>
@@ -1985,10 +2049,13 @@
         <v>160050.0</v>
       </c>
       <c t="s" r="E21">
-        <v>349</v>
-      </c>
-    </row>
-    <row spans="1:6" r="22">
+        <v>350</v>
+      </c>
+      <c t="s" r="F21">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="22">
       <c t="s" r="A22">
         <v>136</v>
       </c>
@@ -2002,15 +2069,18 @@
         <v>80995.0</v>
       </c>
       <c t="s" r="E22">
-        <v>349</v>
-      </c>
-    </row>
-    <row spans="1:6" r="23">
+        <v>350</v>
+      </c>
+      <c t="s" r="F22">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="23">
       <c t="s" r="A23">
         <v>8</v>
       </c>
       <c t="s" r="B23">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c t="s" r="C23">
         <v>86</v>
@@ -2019,15 +2089,18 @@
         <v>384000.0</v>
       </c>
       <c t="s" r="E23">
-        <v>349</v>
-      </c>
-    </row>
-    <row spans="1:6" r="24">
+        <v>350</v>
+      </c>
+      <c t="s" r="F23">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="24">
       <c t="s" r="A24">
         <v>38</v>
       </c>
       <c t="s" r="B24">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c t="s" r="C24">
         <v>9</v>
@@ -2036,10 +2109,13 @@
         <v>576000.0</v>
       </c>
       <c t="s" r="E24">
-        <v>349</v>
-      </c>
-    </row>
-    <row spans="1:6" r="25">
+        <v>350</v>
+      </c>
+      <c t="s" r="F24">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="25">
       <c t="s" r="A25">
         <v>132</v>
       </c>
@@ -2053,10 +2129,13 @@
         <v>225750.0</v>
       </c>
       <c t="s" r="E25">
-        <v>349</v>
-      </c>
-    </row>
-    <row spans="1:6" r="26">
+        <v>350</v>
+      </c>
+      <c t="s" r="F25">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="26">
       <c t="s" r="A26">
         <v>301</v>
       </c>
@@ -2070,10 +2149,13 @@
         <v>340000.0</v>
       </c>
       <c t="s" r="E26">
-        <v>349</v>
-      </c>
-    </row>
-    <row spans="1:6" r="27">
+        <v>350</v>
+      </c>
+      <c t="s" r="F26">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="27">
       <c t="s" r="A27">
         <v>50</v>
       </c>
@@ -2087,10 +2169,13 @@
         <v>225750.0</v>
       </c>
       <c t="s" r="E27">
-        <v>349</v>
-      </c>
-    </row>
-    <row spans="1:6" r="28">
+        <v>350</v>
+      </c>
+      <c t="s" r="F27">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="28">
       <c t="s" r="A28">
         <v>0</v>
       </c>
@@ -2104,10 +2189,13 @@
         <v>823150.0</v>
       </c>
       <c t="s" r="E28">
-        <v>349</v>
-      </c>
-    </row>
-    <row spans="1:6" r="29">
+        <v>350</v>
+      </c>
+      <c t="s" r="F28">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="29">
       <c t="s" r="A29">
         <v>256</v>
       </c>
@@ -2121,10 +2209,13 @@
         <v>365400.0</v>
       </c>
       <c t="s" r="E29">
-        <v>349</v>
-      </c>
-    </row>
-    <row spans="1:6" r="30">
+        <v>350</v>
+      </c>
+      <c t="s" r="F29">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="30">
       <c t="s" r="A30">
         <v>141</v>
       </c>
@@ -2138,10 +2229,13 @@
         <v>379000.0</v>
       </c>
       <c t="s" r="E30">
-        <v>349</v>
-      </c>
-    </row>
-    <row spans="1:6" r="31">
+        <v>350</v>
+      </c>
+      <c t="s" r="F30">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="31">
       <c t="s" r="A31">
         <v>49</v>
       </c>
@@ -2155,10 +2249,13 @@
         <v>209000.0</v>
       </c>
       <c t="s" r="E31">
-        <v>349</v>
-      </c>
-    </row>
-    <row spans="1:6" r="32">
+        <v>350</v>
+      </c>
+      <c t="s" r="F31">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="32">
       <c t="s" r="A32">
         <v>219</v>
       </c>
@@ -2172,10 +2269,13 @@
         <v>730800.0</v>
       </c>
       <c t="s" r="E32">
-        <v>349</v>
-      </c>
-    </row>
-    <row spans="1:6" r="33">
+        <v>350</v>
+      </c>
+      <c t="s" r="F32">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="33">
       <c t="s" r="A33">
         <v>330</v>
       </c>
@@ -2189,10 +2289,13 @@
         <v>340000.0</v>
       </c>
       <c t="s" r="E33">
-        <v>349</v>
-      </c>
-    </row>
-    <row spans="1:6" r="34">
+        <v>350</v>
+      </c>
+      <c t="s" r="F33">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="34">
       <c t="s" r="A34">
         <v>133</v>
       </c>
@@ -2206,10 +2309,13 @@
         <v>78750.0</v>
       </c>
       <c t="s" r="E34">
-        <v>349</v>
-      </c>
-    </row>
-    <row spans="1:6" r="35">
+        <v>350</v>
+      </c>
+      <c t="s" r="F34">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="35">
       <c t="s" r="A35">
         <v>271</v>
       </c>
@@ -2223,12 +2329,15 @@
         <v>1646300.0</v>
       </c>
       <c t="s" r="E35">
-        <v>349</v>
-      </c>
-    </row>
-    <row spans="1:6" r="36">
+        <v>350</v>
+      </c>
+      <c t="s" r="F35">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="36">
       <c t="s" r="A36">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c t="s" r="B36">
         <v>195</v>
@@ -2240,10 +2349,13 @@
         <v>218400.0</v>
       </c>
       <c t="s" r="E36">
-        <v>349</v>
-      </c>
-    </row>
-    <row spans="1:6" r="37">
+        <v>350</v>
+      </c>
+      <c t="s" r="F36">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="37">
       <c t="s" r="A37">
         <v>324</v>
       </c>
@@ -2257,12 +2369,15 @@
         <v>157500.0</v>
       </c>
       <c t="s" r="E37">
-        <v>349</v>
-      </c>
-    </row>
-    <row spans="1:6" r="38">
+        <v>350</v>
+      </c>
+      <c t="s" r="F37">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="38">
       <c t="s" r="A38">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c t="s" r="B38">
         <v>157</v>
@@ -2274,12 +2389,15 @@
         <v>147000.0</v>
       </c>
       <c t="s" r="E38">
-        <v>349</v>
-      </c>
-    </row>
-    <row spans="1:6" r="39">
+        <v>350</v>
+      </c>
+      <c t="s" r="F38">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="39">
       <c t="s" r="A39">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c t="s" r="B39">
         <v>59</v>
@@ -2291,10 +2409,13 @@
         <v>660000.0</v>
       </c>
       <c t="s" r="E39">
-        <v>349</v>
-      </c>
-    </row>
-    <row spans="1:6" r="40">
+        <v>350</v>
+      </c>
+      <c t="s" r="F39">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="40">
       <c t="s" r="A40">
         <v>330</v>
       </c>
@@ -2308,10 +2429,13 @@
         <v>794620.0</v>
       </c>
       <c t="s" r="E40">
-        <v>349</v>
-      </c>
-    </row>
-    <row spans="1:6" r="41">
+        <v>350</v>
+      </c>
+      <c t="s" r="F40">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="41">
       <c t="s" r="A41">
         <v>327</v>
       </c>
@@ -2325,15 +2449,18 @@
         <v>60000.0</v>
       </c>
       <c t="s" r="E41">
-        <v>349</v>
-      </c>
-    </row>
-    <row spans="1:6" r="42">
+        <v>350</v>
+      </c>
+      <c t="s" r="F41">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="42">
       <c t="s" r="A42">
         <v>112</v>
       </c>
       <c t="s" r="B42">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c t="s" r="C42">
         <v>94</v>
@@ -2342,10 +2469,13 @@
         <v>268000.0</v>
       </c>
       <c t="s" r="E42">
-        <v>349</v>
-      </c>
-    </row>
-    <row spans="1:6" r="43">
+        <v>350</v>
+      </c>
+      <c t="s" r="F42">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="43">
       <c t="s" r="A43">
         <v>112</v>
       </c>
@@ -2359,15 +2489,18 @@
         <v>94500.0</v>
       </c>
       <c t="s" r="E43">
-        <v>349</v>
-      </c>
-    </row>
-    <row spans="1:6" r="44">
+        <v>350</v>
+      </c>
+      <c t="s" r="F43">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="44">
       <c t="s" r="A44">
         <v>138</v>
       </c>
       <c t="s" r="B44">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c t="s" r="C44">
         <v>2</v>
@@ -2376,15 +2509,18 @@
         <v>140000.0</v>
       </c>
       <c t="s" r="E44">
-        <v>349</v>
-      </c>
-    </row>
-    <row spans="1:6" r="45">
+        <v>350</v>
+      </c>
+      <c t="s" r="F44">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="45">
       <c t="s" r="A45">
         <v>138</v>
       </c>
       <c t="s" r="B45">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c t="s" r="C45">
         <v>32</v>
@@ -2393,10 +2529,13 @@
         <v>570000.0</v>
       </c>
       <c t="s" r="E45">
-        <v>349</v>
-      </c>
-    </row>
-    <row spans="1:6" r="46">
+        <v>350</v>
+      </c>
+      <c t="s" r="F45">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="46">
       <c t="s" r="A46">
         <v>252</v>
       </c>
@@ -2410,15 +2549,18 @@
         <v>400000.0</v>
       </c>
       <c t="s" r="E46">
-        <v>349</v>
-      </c>
-    </row>
-    <row spans="1:6" r="47">
+        <v>350</v>
+      </c>
+      <c t="s" r="F46">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="47">
       <c t="s" r="A47">
         <v>252</v>
       </c>
       <c t="s" r="B47">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c t="s" r="C47">
         <v>32</v>
@@ -2427,10 +2569,13 @@
         <v>2600000.0</v>
       </c>
       <c t="s" r="E47">
-        <v>349</v>
-      </c>
-    </row>
-    <row spans="1:6" r="48">
+        <v>350</v>
+      </c>
+      <c t="s" r="F47">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="48">
       <c t="s" r="A48">
         <v>252</v>
       </c>
@@ -2444,10 +2589,13 @@
         <v>500000.0</v>
       </c>
       <c t="s" r="E48">
-        <v>349</v>
-      </c>
-    </row>
-    <row spans="1:6" r="49">
+        <v>350</v>
+      </c>
+      <c t="s" r="F48">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="49">
       <c t="s" r="A49">
         <v>252</v>
       </c>
@@ -2461,10 +2609,13 @@
         <v>1370000.0</v>
       </c>
       <c t="s" r="E49">
-        <v>349</v>
-      </c>
-    </row>
-    <row spans="1:6" r="50">
+        <v>350</v>
+      </c>
+      <c t="s" r="F49">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="50">
       <c t="s" r="A50">
         <v>51</v>
       </c>
@@ -2478,10 +2629,13 @@
         <v>905000.0</v>
       </c>
       <c t="s" r="E50">
-        <v>349</v>
-      </c>
-    </row>
-    <row spans="1:6" r="51">
+        <v>350</v>
+      </c>
+      <c t="s" r="F50">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="51">
       <c t="s" r="A51">
         <v>140</v>
       </c>
@@ -2495,10 +2649,13 @@
         <v>1780000.0</v>
       </c>
       <c t="s" r="E51">
-        <v>349</v>
-      </c>
-    </row>
-    <row spans="1:6" r="52">
+        <v>350</v>
+      </c>
+      <c t="s" r="F51">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="52">
       <c t="s" r="A52">
         <v>140</v>
       </c>
@@ -2512,15 +2669,18 @@
         <v>0.0</v>
       </c>
       <c t="s" r="E52">
-        <v>349</v>
-      </c>
-    </row>
-    <row spans="1:6" r="53">
+        <v>350</v>
+      </c>
+      <c t="s" r="F52">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="53">
       <c t="s" r="A53">
         <v>210</v>
       </c>
       <c t="s" r="B53">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c t="s" r="C53">
         <v>32</v>
@@ -2531,8 +2691,11 @@
       <c t="s" r="E53">
         <v>137</v>
       </c>
-    </row>
-    <row spans="1:6" r="54">
+      <c t="s" r="F53">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="54">
       <c t="s" r="A54">
         <v>211</v>
       </c>
@@ -2548,8 +2711,11 @@
       <c t="s" r="E54">
         <v>137</v>
       </c>
-    </row>
-    <row spans="1:6" r="55">
+      <c t="s" r="F54">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="55">
       <c t="s" r="A55">
         <v>214</v>
       </c>
@@ -2565,8 +2731,11 @@
       <c t="s" r="E55">
         <v>137</v>
       </c>
-    </row>
-    <row spans="1:6" r="56">
+      <c t="s" r="F55">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="56">
       <c t="s" r="A56">
         <v>215</v>
       </c>
@@ -2582,8 +2751,11 @@
       <c t="s" r="E56">
         <v>137</v>
       </c>
-    </row>
-    <row spans="1:6" r="57">
+      <c t="s" r="F56">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="57">
       <c t="s" r="A57">
         <v>215</v>
       </c>
@@ -2599,8 +2771,11 @@
       <c t="s" r="E57">
         <v>137</v>
       </c>
-    </row>
-    <row spans="1:6" r="58">
+      <c t="s" r="F57">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="58">
       <c t="s" r="A58">
         <v>215</v>
       </c>
@@ -2616,13 +2791,16 @@
       <c t="s" r="E58">
         <v>137</v>
       </c>
-    </row>
-    <row spans="1:6" r="59">
+      <c t="s" r="F58">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="59">
       <c t="s" r="A59">
         <v>331</v>
       </c>
       <c t="s" r="B59">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c t="s" r="C59">
         <v>39</v>
@@ -2631,10 +2809,13 @@
         <v>100000.0</v>
       </c>
       <c t="s" r="E59">
-        <v>349</v>
-      </c>
-    </row>
-    <row spans="1:6" r="60">
+        <v>350</v>
+      </c>
+      <c t="s" r="F59">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="60">
       <c t="s" r="A60">
         <v>331</v>
       </c>
@@ -2648,10 +2829,13 @@
         <v>460000.0</v>
       </c>
       <c t="s" r="E60">
-        <v>349</v>
-      </c>
-    </row>
-    <row spans="1:6" r="61">
+        <v>350</v>
+      </c>
+      <c t="s" r="F60">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="61">
       <c t="s" r="A61">
         <v>331</v>
       </c>
@@ -2665,12 +2849,15 @@
         <v>160000.0</v>
       </c>
       <c t="s" r="E61">
-        <v>349</v>
-      </c>
-    </row>
-    <row spans="1:6" r="62">
+        <v>350</v>
+      </c>
+      <c t="s" r="F61">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="62">
       <c t="s" r="A62">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c t="s" r="B62">
         <v>197</v>
@@ -2682,15 +2869,18 @@
         <v>300000.0</v>
       </c>
       <c t="s" r="E62">
-        <v>349</v>
-      </c>
-    </row>
-    <row spans="1:6" r="63">
+        <v>350</v>
+      </c>
+      <c t="s" r="F62">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="63">
       <c t="s" r="A63">
         <v>331</v>
       </c>
       <c t="s" r="B63">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c t="s" r="C63">
         <v>9</v>
@@ -2699,10 +2889,13 @@
         <v>1000000.0</v>
       </c>
       <c t="s" r="E63">
-        <v>349</v>
-      </c>
-    </row>
-    <row spans="1:6" r="64">
+        <v>350</v>
+      </c>
+      <c t="s" r="F63">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="64">
       <c t="s" r="A64">
         <v>331</v>
       </c>
@@ -2716,10 +2909,13 @@
         <v>600000.0</v>
       </c>
       <c t="s" r="E64">
-        <v>349</v>
-      </c>
-    </row>
-    <row spans="1:6" r="65">
+        <v>350</v>
+      </c>
+      <c t="s" r="F64">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="65">
       <c t="s" r="A65">
         <v>331</v>
       </c>
@@ -2733,10 +2929,13 @@
         <v>70000.0</v>
       </c>
       <c t="s" r="E65">
-        <v>349</v>
-      </c>
-    </row>
-    <row spans="1:6" r="66">
+        <v>350</v>
+      </c>
+      <c t="s" r="F65">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="66">
       <c t="s" r="A66">
         <v>52</v>
       </c>
@@ -2750,15 +2949,18 @@
         <v>693000.0</v>
       </c>
       <c t="s" r="E66">
-        <v>349</v>
-      </c>
-    </row>
-    <row spans="1:6" r="67">
+        <v>350</v>
+      </c>
+      <c t="s" r="F66">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="67">
       <c t="s" r="A67">
         <v>52</v>
       </c>
       <c t="s" r="B67">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c t="s" r="C67">
         <v>35</v>
@@ -2767,10 +2969,13 @@
         <v>126000.0</v>
       </c>
       <c t="s" r="E67">
-        <v>349</v>
-      </c>
-    </row>
-    <row spans="1:6" r="68">
+        <v>350</v>
+      </c>
+      <c t="s" r="F67">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="68">
       <c t="s" r="A68">
         <v>52</v>
       </c>
@@ -2784,10 +2989,13 @@
         <v>80000.0</v>
       </c>
       <c t="s" r="E68">
-        <v>349</v>
-      </c>
-    </row>
-    <row spans="1:6" r="69">
+        <v>350</v>
+      </c>
+      <c t="s" r="F68">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="69">
       <c t="s" r="A69">
         <v>52</v>
       </c>
@@ -2801,15 +3009,18 @@
         <v>140000.0</v>
       </c>
       <c t="s" r="E69">
-        <v>349</v>
-      </c>
-    </row>
-    <row spans="1:6" r="70">
+        <v>350</v>
+      </c>
+      <c t="s" r="F69">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="70">
       <c t="s" r="A70">
         <v>52</v>
       </c>
       <c t="s" r="B70">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c t="s" r="C70">
         <v>35</v>
@@ -2818,10 +3029,13 @@
         <v>30000.0</v>
       </c>
       <c t="s" r="E70">
-        <v>349</v>
-      </c>
-    </row>
-    <row spans="1:6" r="71">
+        <v>350</v>
+      </c>
+      <c t="s" r="F70">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="71">
       <c t="s" r="A71">
         <v>27</v>
       </c>
@@ -2835,10 +3049,13 @@
         <v>18480.0</v>
       </c>
       <c t="s" r="E71">
-        <v>349</v>
-      </c>
-    </row>
-    <row spans="1:6" r="72">
+        <v>350</v>
+      </c>
+      <c t="s" r="F71">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="72">
       <c t="s" r="A72">
         <v>28</v>
       </c>
@@ -2852,10 +3069,13 @@
         <v>123500.0</v>
       </c>
       <c t="s" r="E72">
-        <v>349</v>
-      </c>
-    </row>
-    <row spans="1:6" r="73">
+        <v>350</v>
+      </c>
+      <c t="s" r="F72">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="73">
       <c t="s" r="A73">
         <v>46</v>
       </c>
@@ -2869,10 +3089,13 @@
         <v>20000.0</v>
       </c>
       <c t="s" r="E73">
-        <v>349</v>
-      </c>
-    </row>
-    <row spans="1:6" r="74">
+        <v>350</v>
+      </c>
+      <c t="s" r="F73">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="74">
       <c t="s" r="A74">
         <v>329</v>
       </c>
@@ -2886,15 +3109,18 @@
         <v>0.0</v>
       </c>
       <c t="s" r="E74">
-        <v>349</v>
-      </c>
-    </row>
-    <row spans="1:6" r="75">
+        <v>350</v>
+      </c>
+      <c t="s" r="F74">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="75">
       <c t="s" r="A75">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c t="s" r="B75">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c t="s" r="C75">
         <v>1</v>
@@ -2905,10 +3131,13 @@
       <c t="s" r="E75">
         <v>258</v>
       </c>
-    </row>
-    <row spans="1:6" r="76">
+      <c t="s" r="F75">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="76">
       <c t="s" r="A76">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c t="s" r="B76">
         <v>163</v>
@@ -2922,10 +3151,13 @@
       <c t="s" r="E76">
         <v>258</v>
       </c>
-    </row>
-    <row spans="1:6" r="77">
+      <c t="s" r="F76">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="77">
       <c t="s" r="A77">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c t="s" r="B77">
         <v>319</v>
@@ -2939,10 +3171,13 @@
       <c t="s" r="E77">
         <v>258</v>
       </c>
-    </row>
-    <row spans="1:6" r="78">
+      <c t="s" r="F77">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="78">
       <c t="s" r="A78">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c t="s" r="B78">
         <v>249</v>
@@ -2956,13 +3191,16 @@
       <c t="s" r="E78">
         <v>258</v>
       </c>
-    </row>
-    <row spans="1:6" r="79">
+      <c t="s" r="F78">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="79">
       <c t="s" r="A79">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c t="s" r="B79">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c t="s" r="C79">
         <v>5</v>
@@ -2973,13 +3211,16 @@
       <c t="s" r="E79">
         <v>258</v>
       </c>
-    </row>
-    <row spans="1:6" r="80">
+      <c t="s" r="F79">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="80">
       <c t="s" r="A80">
         <v>325</v>
       </c>
       <c t="s" r="B80">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c t="s" r="C80">
         <v>43</v>
@@ -2990,8 +3231,11 @@
       <c t="s" r="E80">
         <v>258</v>
       </c>
-    </row>
-    <row spans="1:6" r="81">
+      <c t="s" r="F80">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="81">
       <c t="s" r="A81">
         <v>325</v>
       </c>
@@ -3007,8 +3251,11 @@
       <c t="s" r="E81">
         <v>258</v>
       </c>
-    </row>
-    <row spans="1:6" r="82">
+      <c t="s" r="F81">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="82">
       <c t="s" r="A82">
         <v>325</v>
       </c>
@@ -3024,13 +3271,16 @@
       <c t="s" r="E82">
         <v>258</v>
       </c>
-    </row>
-    <row spans="1:6" r="83">
+      <c t="s" r="F82">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="83">
       <c t="s" r="A83">
         <v>261</v>
       </c>
       <c t="s" r="B83">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c t="s" r="C83">
         <v>55</v>
@@ -3041,8 +3291,11 @@
       <c t="s" r="E83">
         <v>258</v>
       </c>
-    </row>
-    <row spans="1:6" r="84">
+      <c t="s" r="F83">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="84">
       <c t="s" r="A84">
         <v>261</v>
       </c>
@@ -3058,13 +3311,16 @@
       <c t="s" r="E84">
         <v>258</v>
       </c>
-    </row>
-    <row spans="1:6" r="85">
+      <c t="s" r="F84">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="85">
       <c t="s" r="A85">
         <v>261</v>
       </c>
       <c t="s" r="B85">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c t="s" r="C85">
         <v>61</v>
@@ -3075,8 +3331,11 @@
       <c t="s" r="E85">
         <v>258</v>
       </c>
-    </row>
-    <row spans="1:6" r="86">
+      <c t="s" r="F85">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="86">
       <c t="s" r="A86">
         <v>261</v>
       </c>
@@ -3092,8 +3351,11 @@
       <c t="s" r="E86">
         <v>258</v>
       </c>
-    </row>
-    <row spans="1:6" r="87">
+      <c t="s" r="F86">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="87">
       <c t="s" r="A87">
         <v>261</v>
       </c>
@@ -3109,13 +3371,16 @@
       <c t="s" r="E87">
         <v>258</v>
       </c>
-    </row>
-    <row spans="1:6" r="88">
+      <c t="s" r="F87">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="88">
       <c t="s" r="A88">
         <v>143</v>
       </c>
       <c t="s" r="B88">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c t="s" r="C88">
         <v>76</v>
@@ -3126,8 +3391,11 @@
       <c t="s" r="E88">
         <v>258</v>
       </c>
-    </row>
-    <row spans="1:6" r="89">
+      <c t="s" r="F88">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="89">
       <c t="s" r="A89">
         <v>143</v>
       </c>
@@ -3138,13 +3406,16 @@
         <v>64</v>
       </c>
       <c t="n" r="D89">
-        <v>129500.0</v>
+        <v>0.0</v>
       </c>
       <c t="s" r="E89">
         <v>258</v>
       </c>
-    </row>
-    <row spans="1:6" r="90">
+      <c t="s" r="F89">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="90">
       <c t="s" r="A90">
         <v>143</v>
       </c>
@@ -3160,8 +3431,11 @@
       <c t="s" r="E90">
         <v>258</v>
       </c>
-    </row>
-    <row spans="1:6" r="91">
+      <c t="s" r="F90">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="91">
       <c t="s" r="A91">
         <v>143</v>
       </c>
@@ -3177,13 +3451,16 @@
       <c t="s" r="E91">
         <v>258</v>
       </c>
-    </row>
-    <row spans="1:6" r="92">
+      <c t="s" r="F91">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="92">
       <c t="s" r="A92">
         <v>143</v>
       </c>
       <c t="s" r="B92">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c t="s" r="C92">
         <v>95</v>
@@ -3194,8 +3471,11 @@
       <c t="s" r="E92">
         <v>258</v>
       </c>
-    </row>
-    <row spans="1:6" r="93">
+      <c t="s" r="F92">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="93">
       <c t="s" r="A93">
         <v>295</v>
       </c>
@@ -3211,8 +3491,11 @@
       <c t="s" r="E93">
         <v>258</v>
       </c>
-    </row>
-    <row spans="1:6" r="94">
+      <c t="s" r="F93">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="94">
       <c t="s" r="A94">
         <v>295</v>
       </c>
@@ -3228,8 +3511,11 @@
       <c t="s" r="E94">
         <v>258</v>
       </c>
-    </row>
-    <row spans="1:6" r="95">
+      <c t="s" r="F94">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="95">
       <c t="s" r="A95">
         <v>220</v>
       </c>
@@ -3245,13 +3531,16 @@
       <c t="s" r="E95">
         <v>258</v>
       </c>
-    </row>
-    <row spans="1:6" r="96">
+      <c t="s" r="F95">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="96">
       <c t="s" r="A96">
         <v>220</v>
       </c>
       <c t="s" r="B96">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c t="s" r="C96">
         <v>35</v>
@@ -3262,8 +3551,11 @@
       <c t="s" r="E96">
         <v>258</v>
       </c>
-    </row>
-    <row spans="1:6" r="97">
+      <c t="s" r="F96">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="97">
       <c t="s" r="A97">
         <v>220</v>
       </c>
@@ -3279,8 +3571,11 @@
       <c t="s" r="E97">
         <v>258</v>
       </c>
-    </row>
-    <row spans="1:6" r="98">
+      <c t="s" r="F97">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="98">
       <c t="s" r="A98">
         <v>259</v>
       </c>
@@ -3296,8 +3591,11 @@
       <c t="s" r="E98">
         <v>258</v>
       </c>
-    </row>
-    <row spans="1:6" r="99">
+      <c t="s" r="F98">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="99">
       <c t="s" r="A99">
         <v>259</v>
       </c>
@@ -3313,13 +3611,16 @@
       <c t="s" r="E99">
         <v>258</v>
       </c>
-    </row>
-    <row spans="1:6" r="100">
+      <c t="s" r="F99">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="100">
       <c t="s" r="A100">
         <v>259</v>
       </c>
       <c t="s" r="B100">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c t="s" r="C100">
         <v>35</v>
@@ -3330,13 +3631,16 @@
       <c t="s" r="E100">
         <v>258</v>
       </c>
-    </row>
-    <row spans="1:6" r="101">
+      <c t="s" r="F100">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="101">
       <c t="s" r="A101">
         <v>259</v>
       </c>
       <c t="s" r="B101">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c t="s" r="C101">
         <v>39</v>
@@ -3347,8 +3651,11 @@
       <c t="s" r="E101">
         <v>258</v>
       </c>
-    </row>
-    <row spans="1:6" r="102">
+      <c t="s" r="F101">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="102">
       <c t="s" r="A102">
         <v>259</v>
       </c>
@@ -3364,13 +3671,16 @@
       <c t="s" r="E102">
         <v>258</v>
       </c>
-    </row>
-    <row spans="1:6" r="103">
+      <c t="s" r="F102">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="103">
       <c t="s" r="A103">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c t="s" r="B103">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c t="s" r="C103">
         <v>40</v>
@@ -3381,518 +3691,611 @@
       <c t="s" r="E103">
         <v>276</v>
       </c>
-    </row>
-    <row spans="1:6" r="104">
+      <c t="s" r="F103">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="104">
       <c t="s" r="A104">
         <v>111</v>
       </c>
       <c t="s" r="B104">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c t="s" r="C104">
         <v>40</v>
       </c>
       <c t="n" r="D104">
-        <v>3399110.0</v>
+        <v>0.0</v>
       </c>
       <c t="s" r="E104">
         <v>276</v>
       </c>
-    </row>
-    <row spans="1:6" r="105">
+      <c t="s" r="F104">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="105">
       <c t="s" r="A105">
         <v>279</v>
       </c>
       <c t="s" r="B105">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c t="s" r="C105">
         <v>40</v>
       </c>
       <c t="n" r="D105">
-        <v>3399110.0</v>
+        <v>0.0</v>
       </c>
       <c t="s" r="E105">
         <v>276</v>
       </c>
-    </row>
-    <row spans="1:6" r="106">
+      <c t="s" r="F105">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="106">
       <c t="s" r="A106">
         <v>282</v>
       </c>
       <c t="s" r="B106">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c t="s" r="C106">
         <v>40</v>
       </c>
       <c t="n" r="D106">
-        <v>3399110.0</v>
+        <v>0.0</v>
       </c>
       <c t="s" r="E106">
         <v>276</v>
       </c>
-    </row>
-    <row spans="1:6" r="107">
+      <c t="s" r="F106">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="107">
       <c t="s" r="A107">
         <v>260</v>
       </c>
       <c t="s" r="B107">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c t="s" r="C107">
         <v>40</v>
       </c>
       <c t="n" r="D107">
-        <v>3399110.0</v>
+        <v>0.0</v>
       </c>
       <c t="s" r="E107">
         <v>276</v>
       </c>
-    </row>
-    <row spans="1:6" r="108">
+      <c t="s" r="F107">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="108">
       <c t="s" r="A108">
         <v>284</v>
       </c>
       <c t="s" r="B108">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c t="s" r="C108">
         <v>40</v>
       </c>
       <c t="n" r="D108">
-        <v>3399110.0</v>
+        <v>0.0</v>
       </c>
       <c t="s" r="E108">
         <v>276</v>
       </c>
-    </row>
-    <row spans="1:6" r="109">
+      <c t="s" r="F108">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="109">
       <c t="s" r="A109">
         <v>122</v>
       </c>
       <c t="s" r="B109">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c t="s" r="C109">
         <v>40</v>
       </c>
       <c t="n" r="D109">
-        <v>3399110.0</v>
+        <v>0.0</v>
       </c>
       <c t="s" r="E109">
         <v>276</v>
       </c>
-    </row>
-    <row spans="1:6" r="110">
+      <c t="s" r="F109">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="110">
       <c t="s" r="A110">
         <v>268</v>
       </c>
       <c t="s" r="B110">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c t="s" r="C110">
         <v>40</v>
       </c>
       <c t="n" r="D110">
-        <v>3399110.0</v>
+        <v>0.0</v>
       </c>
       <c t="s" r="E110">
         <v>276</v>
       </c>
-    </row>
-    <row spans="1:6" r="111">
+      <c t="s" r="F110">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="111">
       <c t="s" r="A111">
         <v>23</v>
       </c>
       <c t="s" r="B111">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c t="s" r="C111">
         <v>40</v>
       </c>
       <c t="n" r="D111">
-        <v>3399110.0</v>
+        <v>0.0</v>
       </c>
       <c t="s" r="E111">
         <v>276</v>
       </c>
-    </row>
-    <row spans="1:6" r="112">
+      <c t="s" r="F111">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="112">
       <c t="s" r="A112">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c t="s" r="B112">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c t="s" r="C112">
         <v>40</v>
       </c>
       <c t="n" r="D112">
-        <v>3399110.0</v>
+        <v>0.0</v>
       </c>
       <c t="s" r="E112">
         <v>276</v>
       </c>
-    </row>
-    <row spans="1:6" r="113">
+      <c t="s" r="F112">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="113">
       <c t="s" r="A113">
         <v>121</v>
       </c>
       <c t="s" r="B113">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c t="s" r="C113">
         <v>40</v>
       </c>
       <c t="n" r="D113">
-        <v>3399110.0</v>
+        <v>0.0</v>
       </c>
       <c t="s" r="E113">
         <v>276</v>
       </c>
-    </row>
-    <row spans="1:6" r="114">
+      <c t="s" r="F113">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="114">
       <c t="s" r="A114">
         <v>278</v>
       </c>
       <c t="s" r="B114">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c t="s" r="C114">
         <v>40</v>
       </c>
       <c t="n" r="D114">
-        <v>3399110.0</v>
+        <v>0.0</v>
       </c>
       <c t="s" r="E114">
         <v>276</v>
       </c>
-    </row>
-    <row spans="1:6" r="115">
+      <c t="s" r="F114">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="115">
       <c t="s" r="A115">
         <v>213</v>
       </c>
       <c t="s" r="B115">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c t="s" r="C115">
         <v>40</v>
       </c>
       <c t="n" r="D115">
-        <v>3399110.0</v>
+        <v>0.0</v>
       </c>
       <c t="s" r="E115">
         <v>276</v>
       </c>
-    </row>
-    <row spans="1:6" r="116">
+      <c t="s" r="F115">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="116">
       <c t="s" r="A116">
         <v>24</v>
       </c>
       <c t="s" r="B116">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c t="s" r="C116">
         <v>40</v>
       </c>
       <c t="n" r="D116">
-        <v>3399110.0</v>
+        <v>0.0</v>
       </c>
       <c t="s" r="E116">
         <v>276</v>
       </c>
-    </row>
-    <row spans="1:6" r="117">
+      <c t="s" r="F116">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="117">
       <c t="s" r="A117">
         <v>273</v>
       </c>
       <c t="s" r="B117">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c t="s" r="C117">
         <v>40</v>
       </c>
       <c t="n" r="D117">
-        <v>3399110.0</v>
+        <v>0.0</v>
       </c>
       <c t="s" r="E117">
         <v>276</v>
       </c>
-    </row>
-    <row spans="1:6" r="118">
+      <c t="s" r="F117">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="118">
       <c t="s" r="A118">
         <v>273</v>
       </c>
       <c t="s" r="B118">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c t="s" r="C118">
         <v>40</v>
       </c>
       <c t="n" r="D118">
-        <v>3399110.0</v>
+        <v>0.0</v>
       </c>
       <c t="s" r="E118">
         <v>276</v>
       </c>
-    </row>
-    <row spans="1:6" r="119">
+      <c t="s" r="F118">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="119">
       <c t="s" r="A119">
         <v>270</v>
       </c>
       <c t="s" r="B119">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c t="s" r="C119">
         <v>40</v>
       </c>
       <c t="n" r="D119">
-        <v>3399110.0</v>
+        <v>0.0</v>
       </c>
       <c t="s" r="E119">
         <v>276</v>
       </c>
-    </row>
-    <row spans="1:6" r="120">
+      <c t="s" r="F119">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="120">
       <c t="s" r="A120">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c t="s" r="B120">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c t="s" r="C120">
         <v>40</v>
       </c>
       <c t="n" r="D120">
-        <v>3399110.0</v>
+        <v>0.0</v>
       </c>
       <c t="s" r="E120">
         <v>276</v>
       </c>
-    </row>
-    <row spans="1:6" r="121">
+      <c t="s" r="F120">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="121">
       <c t="s" r="A121">
         <v>135</v>
       </c>
       <c t="s" r="B121">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c t="s" r="C121">
         <v>40</v>
       </c>
       <c t="n" r="D121">
-        <v>3399110.0</v>
+        <v>0.0</v>
       </c>
       <c t="s" r="E121">
         <v>276</v>
       </c>
-    </row>
-    <row spans="1:6" r="122">
+      <c t="s" r="F121">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="122">
       <c t="s" r="A122">
         <v>332</v>
       </c>
       <c t="s" r="B122">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c t="s" r="C122">
         <v>40</v>
       </c>
       <c t="n" r="D122">
-        <v>3399110.0</v>
+        <v>0.0</v>
       </c>
       <c t="s" r="E122">
         <v>276</v>
       </c>
-    </row>
-    <row spans="1:6" r="123">
+      <c t="s" r="F122">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="123">
       <c t="s" r="A123">
         <v>25</v>
       </c>
       <c t="s" r="B123">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c t="s" r="C123">
         <v>40</v>
       </c>
       <c t="n" r="D123">
-        <v>3399110.0</v>
+        <v>0.0</v>
       </c>
       <c t="s" r="E123">
         <v>276</v>
       </c>
-    </row>
-    <row spans="1:6" r="124">
+      <c t="s" r="F123">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="124">
       <c t="s" r="A124">
         <v>208</v>
       </c>
       <c t="s" r="B124">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c t="s" r="C124">
         <v>40</v>
       </c>
       <c t="n" r="D124">
-        <v>3399110.0</v>
+        <v>0.0</v>
       </c>
       <c t="s" r="E124">
         <v>276</v>
       </c>
-    </row>
-    <row spans="1:6" r="125">
+      <c t="s" r="F124">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="125">
       <c t="s" r="A125">
         <v>280</v>
       </c>
       <c t="s" r="B125">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c t="s" r="C125">
         <v>40</v>
       </c>
       <c t="n" r="D125">
-        <v>3399110.0</v>
+        <v>0.0</v>
       </c>
       <c t="s" r="E125">
         <v>276</v>
       </c>
-    </row>
-    <row spans="1:6" r="126">
+      <c t="s" r="F125">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="126">
       <c t="s" r="A126">
         <v>299</v>
       </c>
       <c t="s" r="B126">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c t="s" r="C126">
         <v>40</v>
       </c>
       <c t="n" r="D126">
-        <v>3399110.0</v>
+        <v>0.0</v>
       </c>
       <c t="s" r="E126">
         <v>276</v>
       </c>
-    </row>
-    <row spans="1:6" r="127">
+      <c t="s" r="F126">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="127">
       <c t="s" r="A127">
         <v>116</v>
       </c>
       <c t="s" r="B127">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c t="s" r="C127">
         <v>40</v>
       </c>
       <c t="n" r="D127">
-        <v>3399110.0</v>
+        <v>0.0</v>
       </c>
       <c t="s" r="E127">
         <v>276</v>
       </c>
-    </row>
-    <row spans="1:6" r="128">
+      <c t="s" r="F127">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="128">
       <c t="s" r="A128">
         <v>250</v>
       </c>
       <c t="s" r="B128">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c t="s" r="C128">
         <v>40</v>
       </c>
       <c t="n" r="D128">
-        <v>3399110.0</v>
+        <v>0.0</v>
       </c>
       <c t="s" r="E128">
         <v>276</v>
       </c>
-    </row>
-    <row spans="1:6" r="129">
+      <c t="s" r="F128">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="129">
       <c t="s" r="A129">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c t="s" r="B129">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c t="s" r="C129">
         <v>40</v>
       </c>
       <c t="n" r="D129">
-        <v>3399110.0</v>
+        <v>0.0</v>
       </c>
       <c t="s" r="E129">
         <v>276</v>
       </c>
-    </row>
-    <row spans="1:6" r="130">
+      <c t="s" r="F129">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="130">
       <c t="s" r="A130">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c t="s" r="B130">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c t="s" r="C130">
         <v>40</v>
       </c>
       <c t="n" r="D130">
-        <v>3399110.0</v>
+        <v>0.0</v>
       </c>
       <c t="s" r="E130">
         <v>276</v>
       </c>
-    </row>
-    <row spans="1:6" r="131">
+      <c t="s" r="F130">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="131">
       <c t="s" r="A131">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c t="s" r="B131">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c t="s" r="C131">
         <v>40</v>
       </c>
       <c t="n" r="D131">
-        <v>3399110.0</v>
+        <v>0.0</v>
       </c>
       <c t="s" r="E131">
         <v>276</v>
       </c>
-    </row>
-    <row spans="1:6" r="132">
+      <c t="s" r="F131">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="132">
       <c t="s" r="A132">
         <v>269</v>
       </c>
       <c t="s" r="B132">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c t="s" r="C132">
         <v>40</v>
       </c>
       <c t="n" r="D132">
-        <v>3399110.0</v>
+        <v>0.0</v>
       </c>
       <c t="s" r="E132">
         <v>276</v>
       </c>
-    </row>
-    <row spans="1:6" r="133">
+      <c t="s" r="F132">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="133">
       <c t="s" r="A133">
         <v>320</v>
       </c>
       <c t="s" r="B133">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c t="s" r="C133">
         <v>40</v>
       </c>
       <c t="n" r="D133">
-        <v>3399110.0</v>
+        <v>0.0</v>
       </c>
       <c t="s" r="E133">
         <v>276</v>
       </c>
-    </row>
-    <row spans="1:6" r="134">
+      <c t="s" r="F133">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="134">
       <c t="s" r="A134">
         <v>116</v>
       </c>
@@ -3908,8 +4311,11 @@
       <c t="s" r="E134">
         <v>276</v>
       </c>
-    </row>
-    <row spans="1:6" r="135">
+      <c t="s" r="F134">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="135">
       <c t="s" r="A135">
         <v>277</v>
       </c>
@@ -3925,8 +4331,11 @@
       <c t="s" r="E135">
         <v>276</v>
       </c>
-    </row>
-    <row spans="1:6" r="136">
+      <c t="s" r="F135">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="136">
       <c t="s" r="A136">
         <v>277</v>
       </c>
@@ -3942,13 +4351,16 @@
       <c t="s" r="E136">
         <v>276</v>
       </c>
-    </row>
-    <row spans="1:6" r="137">
+      <c t="s" r="F136">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="137">
       <c t="s" r="A137">
         <v>292</v>
       </c>
       <c t="s" r="B137">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c t="s" r="C137">
         <v>105</v>
@@ -3959,8 +4371,11 @@
       <c t="s" r="E137">
         <v>276</v>
       </c>
-    </row>
-    <row spans="1:6" r="138">
+      <c t="s" r="F137">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="138">
       <c t="s" r="A138">
         <v>292</v>
       </c>
@@ -3976,13 +4391,16 @@
       <c t="s" r="E138">
         <v>276</v>
       </c>
-    </row>
-    <row spans="1:6" r="139">
+      <c t="s" r="F138">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="139">
       <c t="s" r="A139">
         <v>262</v>
       </c>
       <c t="s" r="B139">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c t="s" r="C139">
         <v>33</v>
@@ -3993,8 +4411,11 @@
       <c t="s" r="E139">
         <v>276</v>
       </c>
-    </row>
-    <row spans="1:6" r="140">
+      <c t="s" r="F139">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="140">
       <c t="s" r="A140">
         <v>262</v>
       </c>
@@ -4010,8 +4431,11 @@
       <c t="s" r="E140">
         <v>276</v>
       </c>
-    </row>
-    <row spans="1:6" r="141">
+      <c t="s" r="F140">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="141">
       <c t="s" r="A141">
         <v>127</v>
       </c>
@@ -4027,13 +4451,16 @@
       <c t="s" r="E141">
         <v>276</v>
       </c>
-    </row>
-    <row spans="1:6" r="142">
+      <c t="s" r="F141">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="142">
       <c t="s" r="A142">
         <v>127</v>
       </c>
       <c t="s" r="B142">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c t="s" r="C142">
         <v>35</v>
@@ -4044,8 +4471,11 @@
       <c t="s" r="E142">
         <v>276</v>
       </c>
-    </row>
-    <row spans="1:6" r="143">
+      <c t="s" r="F142">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="143">
       <c t="s" r="A143">
         <v>291</v>
       </c>
@@ -4061,13 +4491,16 @@
       <c t="s" r="E143">
         <v>276</v>
       </c>
-    </row>
-    <row spans="1:6" r="144">
+      <c t="s" r="F143">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="144">
       <c t="s" r="A144">
         <v>291</v>
       </c>
       <c t="s" r="B144">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c t="s" r="C144">
         <v>35</v>
@@ -4078,10 +4511,13 @@
       <c t="s" r="E144">
         <v>276</v>
       </c>
-    </row>
-    <row spans="1:6" r="145">
+      <c t="s" r="F144">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="145">
       <c t="s" r="A145">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c t="s" r="B145">
         <v>183</v>
@@ -4095,13 +4531,16 @@
       <c t="s" r="E145">
         <v>276</v>
       </c>
-    </row>
-    <row spans="1:6" r="146">
+      <c t="s" r="F145">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="146">
       <c t="s" r="A146">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c t="s" r="B146">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c t="s" r="C146">
         <v>35</v>
@@ -4112,8 +4551,11 @@
       <c t="s" r="E146">
         <v>276</v>
       </c>
-    </row>
-    <row spans="1:6" r="147">
+      <c t="s" r="F146">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="147">
       <c t="s" r="A147">
         <v>281</v>
       </c>
@@ -4129,13 +4571,16 @@
       <c t="s" r="E147">
         <v>276</v>
       </c>
-    </row>
-    <row spans="1:6" r="148">
+      <c t="s" r="F147">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="148">
       <c t="s" r="A148">
         <v>281</v>
       </c>
       <c t="s" r="B148">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c t="s" r="C148">
         <v>35</v>
@@ -4146,13 +4591,16 @@
       <c t="s" r="E148">
         <v>276</v>
       </c>
-    </row>
-    <row spans="1:6" r="149">
+      <c t="s" r="F148">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="149">
       <c t="s" r="A149">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c t="s" r="B149">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c t="s" r="C149">
         <v>77</v>
@@ -4163,13 +4611,16 @@
       <c t="s" r="E149">
         <v>276</v>
       </c>
-    </row>
-    <row spans="1:6" r="150">
+      <c t="s" r="F149">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="150">
       <c t="s" r="A150">
         <v>210</v>
       </c>
       <c t="s" r="B150">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c t="s" r="C150">
         <v>34</v>
@@ -4180,8 +4631,11 @@
       <c t="s" r="E150">
         <v>276</v>
       </c>
-    </row>
-    <row spans="1:6" r="151">
+      <c t="s" r="F150">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="151">
       <c t="s" r="A151">
         <v>274</v>
       </c>
@@ -4197,13 +4651,16 @@
       <c t="s" r="E151">
         <v>276</v>
       </c>
-    </row>
-    <row spans="1:6" r="152">
+      <c t="s" r="F151">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="152">
       <c t="s" r="A152">
         <v>287</v>
       </c>
       <c t="s" r="B152">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c t="s" r="C152">
         <v>69</v>
@@ -4214,13 +4671,16 @@
       <c t="s" r="E152">
         <v>276</v>
       </c>
-    </row>
-    <row spans="1:6" r="153">
+      <c t="s" r="F152">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="153">
       <c t="s" r="A153">
         <v>131</v>
       </c>
       <c t="s" r="B153">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c t="s" r="C153">
         <v>67</v>
@@ -4229,15 +4689,18 @@
         <v>40000.0</v>
       </c>
       <c t="s" r="E153">
-        <v>343</v>
-      </c>
-    </row>
-    <row spans="1:6" r="154">
+        <v>344</v>
+      </c>
+      <c t="s" r="F153">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="154">
       <c t="s" r="A154">
         <v>253</v>
       </c>
       <c t="s" r="B154">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c t="s" r="C154">
         <v>2</v>
@@ -4246,10 +4709,13 @@
         <v>484800.0</v>
       </c>
       <c t="s" r="E154">
-        <v>342</v>
-      </c>
-    </row>
-    <row spans="1:6" r="155">
+        <v>343</v>
+      </c>
+      <c t="s" r="F154">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="155">
       <c t="s" r="A155">
         <v>254</v>
       </c>
@@ -4263,15 +4729,18 @@
         <v>1400000.0</v>
       </c>
       <c t="s" r="E155">
-        <v>342</v>
-      </c>
-    </row>
-    <row spans="1:6" r="156">
+        <v>343</v>
+      </c>
+      <c t="s" r="F155">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="156">
       <c t="s" r="A156">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c t="s" r="B156">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c t="s" r="C156">
         <v>53</v>
@@ -4280,15 +4749,18 @@
         <v>320000.0</v>
       </c>
       <c t="s" r="E156">
-        <v>342</v>
-      </c>
-    </row>
-    <row spans="1:6" r="157">
+        <v>343</v>
+      </c>
+      <c t="s" r="F156">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="157">
       <c t="s" r="A157">
         <v>283</v>
       </c>
       <c t="s" r="B157">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c t="s" r="C157">
         <v>80</v>
@@ -4297,15 +4769,18 @@
         <v>96000.0</v>
       </c>
       <c t="s" r="E157">
-        <v>342</v>
-      </c>
-    </row>
-    <row spans="1:6" r="158">
+        <v>343</v>
+      </c>
+      <c t="s" r="F157">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="158">
       <c t="s" r="A158">
         <v>296</v>
       </c>
       <c t="s" r="B158">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c t="s" r="C158">
         <v>109</v>
@@ -4314,10 +4789,13 @@
         <v>2171000.0</v>
       </c>
       <c t="s" r="E158">
-        <v>342</v>
-      </c>
-    </row>
-    <row spans="1:6" r="159">
+        <v>343</v>
+      </c>
+      <c t="s" r="F158">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="159">
       <c t="s" r="A159">
         <v>296</v>
       </c>
@@ -4331,10 +4809,13 @@
         <v>600000.0</v>
       </c>
       <c t="s" r="E159">
-        <v>342</v>
-      </c>
-    </row>
-    <row spans="1:6" r="160">
+        <v>343</v>
+      </c>
+      <c t="s" r="F159">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="160">
       <c t="s" r="A160">
         <v>130</v>
       </c>
@@ -4348,10 +4829,13 @@
         <v>820600.0</v>
       </c>
       <c t="s" r="E160">
-        <v>342</v>
-      </c>
-    </row>
-    <row spans="1:6" r="161">
+        <v>343</v>
+      </c>
+      <c t="s" r="F160">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="161">
       <c t="s" r="A161">
         <v>130</v>
       </c>
@@ -4365,15 +4849,18 @@
         <v>105000.0</v>
       </c>
       <c t="s" r="E161">
-        <v>342</v>
-      </c>
-    </row>
-    <row spans="1:6" r="162">
+        <v>343</v>
+      </c>
+      <c t="s" r="F161">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="162">
       <c t="s" r="A162">
         <v>115</v>
       </c>
       <c t="s" r="B162">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c t="s" r="C162">
         <v>34</v>
@@ -4382,15 +4869,18 @@
         <v>50400.0</v>
       </c>
       <c t="s" r="E162">
-        <v>342</v>
-      </c>
-    </row>
-    <row spans="1:6" r="163">
+        <v>343</v>
+      </c>
+      <c t="s" r="F162">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="163">
       <c t="s" r="A163">
         <v>290</v>
       </c>
       <c t="s" r="B163">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c t="s" r="C163">
         <v>84</v>
@@ -4399,15 +4889,18 @@
         <v>95000.0</v>
       </c>
       <c t="s" r="E163">
-        <v>342</v>
-      </c>
-    </row>
-    <row spans="1:6" r="164">
+        <v>343</v>
+      </c>
+      <c t="s" r="F163">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="164">
       <c t="s" r="A164">
         <v>298</v>
       </c>
       <c t="s" r="B164">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c t="s" r="C164">
         <v>35</v>
@@ -4416,10 +4909,13 @@
         <v>50000.0</v>
       </c>
       <c t="s" r="E164">
-        <v>342</v>
-      </c>
-    </row>
-    <row spans="1:6" r="165">
+        <v>343</v>
+      </c>
+      <c t="s" r="F164">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="165">
       <c t="s" r="A165">
         <v>294</v>
       </c>
@@ -4433,15 +4929,18 @@
         <v>208500.0</v>
       </c>
       <c t="s" r="E165">
-        <v>342</v>
-      </c>
-    </row>
-    <row spans="1:6" r="166">
+        <v>343</v>
+      </c>
+      <c t="s" r="F165">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="166">
       <c t="s" r="A166">
         <v>289</v>
       </c>
       <c t="s" r="B166">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c t="s" r="C166">
         <v>35</v>
@@ -4450,10 +4949,13 @@
         <v>90000.0</v>
       </c>
       <c t="s" r="E166">
-        <v>342</v>
-      </c>
-    </row>
-    <row spans="1:6" r="167">
+        <v>343</v>
+      </c>
+      <c t="s" r="F166">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="167">
       <c t="s" r="A167">
         <v>289</v>
       </c>
@@ -4467,10 +4969,13 @@
         <v>81000.0</v>
       </c>
       <c t="s" r="E167">
-        <v>342</v>
-      </c>
-    </row>
-    <row spans="1:6" r="168">
+        <v>343</v>
+      </c>
+      <c t="s" r="F167">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="168">
       <c t="s" r="A168">
         <v>116</v>
       </c>
@@ -4484,10 +4989,13 @@
         <v>508800.0</v>
       </c>
       <c t="s" r="E168">
-        <v>341</v>
-      </c>
-    </row>
-    <row spans="1:6" r="169">
+        <v>342</v>
+      </c>
+      <c t="s" r="F168">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="169">
       <c t="s" r="A169">
         <v>292</v>
       </c>
@@ -4501,10 +5009,13 @@
         <v>351000.0</v>
       </c>
       <c t="s" r="E169">
-        <v>341</v>
-      </c>
-    </row>
-    <row spans="1:6" r="170">
+        <v>342</v>
+      </c>
+      <c t="s" r="F169">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="170">
       <c t="s" r="A170">
         <v>127</v>
       </c>
@@ -4518,10 +5029,13 @@
         <v>175500.0</v>
       </c>
       <c t="s" r="E170">
-        <v>341</v>
-      </c>
-    </row>
-    <row spans="1:6" r="171">
+        <v>342</v>
+      </c>
+      <c t="s" r="F170">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="171">
       <c t="s" r="A171">
         <v>262</v>
       </c>
@@ -4535,15 +5049,18 @@
         <v>292500.0</v>
       </c>
       <c t="s" r="E171">
-        <v>341</v>
-      </c>
-    </row>
-    <row spans="1:6" r="172">
+        <v>342</v>
+      </c>
+      <c t="s" r="F171">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="172">
       <c t="s" r="A172">
         <v>266</v>
       </c>
       <c t="s" r="B172">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c t="s" r="C172">
         <v>71</v>
@@ -4554,8 +5071,11 @@
       <c t="s" r="E172">
         <v>264</v>
       </c>
-    </row>
-    <row spans="1:6" r="173">
+      <c t="s" r="F172">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="173">
       <c t="s" r="A173">
         <v>266</v>
       </c>
@@ -4571,8 +5091,11 @@
       <c t="s" r="E173">
         <v>264</v>
       </c>
-    </row>
-    <row spans="1:6" r="174">
+      <c t="s" r="F173">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="174">
       <c t="s" r="A174">
         <v>266</v>
       </c>
@@ -4588,13 +5111,16 @@
       <c t="s" r="E174">
         <v>264</v>
       </c>
-    </row>
-    <row spans="1:6" r="175">
+      <c t="s" r="F174">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="175">
       <c t="s" r="A175">
         <v>147</v>
       </c>
       <c t="s" r="B175">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c t="s" r="C175">
         <v>71</v>
@@ -4605,8 +5131,11 @@
       <c t="s" r="E175">
         <v>264</v>
       </c>
-    </row>
-    <row spans="1:6" r="176">
+      <c t="s" r="F175">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="176">
       <c t="s" r="A176">
         <v>147</v>
       </c>
@@ -4622,8 +5151,11 @@
       <c t="s" r="E176">
         <v>264</v>
       </c>
-    </row>
-    <row spans="1:6" r="177">
+      <c t="s" r="F176">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="177">
       <c t="s" r="A177">
         <v>147</v>
       </c>
@@ -4639,8 +5171,11 @@
       <c t="s" r="E177">
         <v>264</v>
       </c>
-    </row>
-    <row spans="1:6" r="178">
+      <c t="s" r="F177">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="178">
       <c t="s" r="A178">
         <v>147</v>
       </c>
@@ -4656,13 +5191,16 @@
       <c t="s" r="E178">
         <v>264</v>
       </c>
-    </row>
-    <row spans="1:6" r="179">
+      <c t="s" r="F178">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="179">
       <c t="s" r="A179">
         <v>288</v>
       </c>
       <c t="s" r="B179">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c t="s" r="C179">
         <v>87</v>
@@ -4673,8 +5211,11 @@
       <c t="s" r="E179">
         <v>264</v>
       </c>
-    </row>
-    <row spans="1:6" r="180">
+      <c t="s" r="F179">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="180">
       <c t="s" r="A180">
         <v>288</v>
       </c>
@@ -4690,8 +5231,11 @@
       <c t="s" r="E180">
         <v>264</v>
       </c>
-    </row>
-    <row spans="1:6" r="181">
+      <c t="s" r="F180">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="181">
       <c t="s" r="A181">
         <v>288</v>
       </c>
@@ -4707,8 +5251,11 @@
       <c t="s" r="E181">
         <v>264</v>
       </c>
-    </row>
-    <row spans="1:6" r="182">
+      <c t="s" r="F181">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="182">
       <c t="s" r="A182">
         <v>288</v>
       </c>
@@ -4724,13 +5271,16 @@
       <c t="s" r="E182">
         <v>264</v>
       </c>
-    </row>
-    <row spans="1:6" r="183">
+      <c t="s" r="F182">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="183">
       <c t="s" r="A183">
         <v>22</v>
       </c>
       <c t="s" r="B183">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c t="s" r="C183">
         <v>35</v>
@@ -4741,8 +5291,11 @@
       <c t="s" r="E183">
         <v>264</v>
       </c>
-    </row>
-    <row spans="1:6" r="184">
+      <c t="s" r="F183">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="184">
       <c t="s" r="A184">
         <v>22</v>
       </c>
@@ -4758,8 +5311,11 @@
       <c t="s" r="E184">
         <v>264</v>
       </c>
-    </row>
-    <row spans="1:6" r="185">
+      <c t="s" r="F184">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="185">
       <c t="s" r="A185">
         <v>297</v>
       </c>
@@ -4775,8 +5331,11 @@
       <c t="s" r="E185">
         <v>264</v>
       </c>
-    </row>
-    <row spans="1:6" r="186">
+      <c t="s" r="F185">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="186">
       <c t="s" r="A186">
         <v>297</v>
       </c>
@@ -4792,8 +5351,11 @@
       <c t="s" r="E186">
         <v>264</v>
       </c>
-    </row>
-    <row spans="1:6" r="187">
+      <c t="s" r="F186">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="187">
       <c t="s" r="A187">
         <v>265</v>
       </c>
@@ -4809,8 +5371,11 @@
       <c t="s" r="E187">
         <v>264</v>
       </c>
-    </row>
-    <row spans="1:6" r="188">
+      <c t="s" r="F187">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="188">
       <c t="s" r="A188">
         <v>265</v>
       </c>
@@ -4826,8 +5391,11 @@
       <c t="s" r="E188">
         <v>264</v>
       </c>
-    </row>
-    <row spans="1:6" r="189">
+      <c t="s" r="F188">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="189">
       <c t="s" r="A189">
         <v>148</v>
       </c>
@@ -4843,8 +5411,11 @@
       <c t="s" r="E189">
         <v>264</v>
       </c>
-    </row>
-    <row spans="1:6" r="190">
+      <c t="s" r="F189">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="190">
       <c t="s" r="A190">
         <v>148</v>
       </c>
@@ -4860,10 +5431,13 @@
       <c t="s" r="E190">
         <v>264</v>
       </c>
-    </row>
-    <row spans="1:6" r="191">
+      <c t="s" r="F190">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="191">
       <c t="s" r="A191">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c t="s" r="B191">
         <v>309</v>
@@ -4877,10 +5451,13 @@
       <c t="s" r="E191">
         <v>264</v>
       </c>
-    </row>
-    <row spans="1:6" r="192">
+      <c t="s" r="F191">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="192">
       <c t="s" r="A192">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c t="s" r="B192">
         <v>192</v>
@@ -4894,10 +5471,13 @@
       <c t="s" r="E192">
         <v>264</v>
       </c>
-    </row>
-    <row spans="1:6" r="193">
+      <c t="s" r="F192">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="193">
       <c t="s" r="A193">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c t="s" r="B193">
         <v>241</v>
@@ -4911,13 +5491,16 @@
       <c t="s" r="E193">
         <v>264</v>
       </c>
-    </row>
-    <row spans="1:6" r="194">
+      <c t="s" r="F193">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="194">
       <c t="s" r="A194">
         <v>114</v>
       </c>
       <c t="s" r="B194">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c t="s" r="C194">
         <v>87</v>
@@ -4928,8 +5511,11 @@
       <c t="s" r="E194">
         <v>264</v>
       </c>
-    </row>
-    <row spans="1:6" r="195">
+      <c t="s" r="F194">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="195">
       <c t="s" r="A195">
         <v>114</v>
       </c>
@@ -4945,8 +5531,11 @@
       <c t="s" r="E195">
         <v>264</v>
       </c>
-    </row>
-    <row spans="1:6" r="196">
+      <c t="s" r="F195">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="196">
       <c t="s" r="A196">
         <v>114</v>
       </c>
@@ -4962,8 +5551,11 @@
       <c t="s" r="E196">
         <v>264</v>
       </c>
-    </row>
-    <row spans="1:6" r="197">
+      <c t="s" r="F196">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="197">
       <c t="s" r="A197">
         <v>114</v>
       </c>
@@ -4979,13 +5571,16 @@
       <c t="s" r="E197">
         <v>264</v>
       </c>
-    </row>
-    <row spans="1:6" r="198">
+      <c t="s" r="F197">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="198">
       <c t="s" r="A198">
         <v>267</v>
       </c>
       <c t="s" r="B198">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c t="s" r="C198">
         <v>35</v>
@@ -4996,8 +5591,11 @@
       <c t="s" r="E198">
         <v>264</v>
       </c>
-    </row>
-    <row spans="1:6" r="199">
+      <c t="s" r="F198">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="199">
       <c t="s" r="A199">
         <v>267</v>
       </c>
@@ -5013,10 +5611,13 @@
       <c t="s" r="E199">
         <v>264</v>
       </c>
-    </row>
-    <row spans="1:6" r="200">
+      <c t="s" r="F199">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="200">
       <c t="s" r="A200">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c t="s" r="B200">
         <v>240</v>
@@ -5030,8 +5631,11 @@
       <c t="s" r="E200">
         <v>264</v>
       </c>
-    </row>
-    <row spans="1:6" r="201">
+      <c t="s" r="F200">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="201">
       <c t="s" r="A201">
         <v>26</v>
       </c>
@@ -5047,8 +5651,11 @@
       <c t="s" r="E201">
         <v>264</v>
       </c>
-    </row>
-    <row spans="1:6" r="202">
+      <c t="s" r="F201">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="202">
       <c t="s" r="A202">
         <v>26</v>
       </c>
@@ -5064,10 +5671,13 @@
       <c t="s" r="E202">
         <v>264</v>
       </c>
-    </row>
-    <row spans="1:6" r="203">
+      <c t="s" r="F202">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="203">
       <c t="s" r="A203">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c t="s" r="B203">
         <v>174</v>
@@ -5081,10 +5691,13 @@
       <c t="s" r="E203">
         <v>264</v>
       </c>
-    </row>
-    <row spans="1:6" r="204">
+      <c t="s" r="F203">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="204">
       <c t="s" r="A204">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c t="s" r="B204">
         <v>240</v>
@@ -5098,8 +5711,11 @@
       <c t="s" r="E204">
         <v>264</v>
       </c>
-    </row>
-    <row spans="1:6" r="205">
+      <c t="s" r="F204">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="205">
       <c t="s" r="A205">
         <v>212</v>
       </c>
@@ -5113,12 +5729,15 @@
         <v>60000.0</v>
       </c>
       <c t="s" r="E205">
-        <v>358</v>
-      </c>
-    </row>
-    <row spans="1:6" r="206">
+        <v>359</v>
+      </c>
+      <c t="s" r="F205">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="206">
       <c t="s" r="A206">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c t="s" r="B206">
         <v>263</v>
@@ -5130,10 +5749,13 @@
         <v>2470000.0</v>
       </c>
       <c t="s" r="E206">
-        <v>358</v>
-      </c>
-    </row>
-    <row spans="1:6" r="207">
+        <v>359</v>
+      </c>
+      <c t="s" r="F206">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="207">
       <c t="s" r="A207">
         <v>128</v>
       </c>
@@ -5147,15 +5769,18 @@
         <v>96000.0</v>
       </c>
       <c t="s" r="E207">
-        <v>358</v>
-      </c>
-    </row>
-    <row spans="1:6" r="208">
+        <v>359</v>
+      </c>
+      <c t="s" r="F207">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="208">
       <c t="s" r="A208">
         <v>300</v>
       </c>
       <c t="s" r="B208">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c t="s" r="C208">
         <v>10</v>
@@ -5164,10 +5789,13 @@
         <v>88000.0</v>
       </c>
       <c t="s" r="E208">
-        <v>358</v>
-      </c>
-    </row>
-    <row spans="1:6" r="209">
+        <v>359</v>
+      </c>
+      <c t="s" r="F208">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="209">
       <c t="s" r="A209">
         <v>328</v>
       </c>
@@ -5181,10 +5809,13 @@
         <v>850000.0</v>
       </c>
       <c t="s" r="E209">
-        <v>358</v>
-      </c>
-    </row>
-    <row spans="1:6" r="210">
+        <v>359</v>
+      </c>
+      <c t="s" r="F209">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="210">
       <c t="s" r="A210">
         <v>328</v>
       </c>
@@ -5198,15 +5829,18 @@
         <v>190000.0</v>
       </c>
       <c t="s" r="E210">
-        <v>358</v>
-      </c>
-    </row>
-    <row spans="1:6" r="211">
+        <v>359</v>
+      </c>
+      <c t="s" r="F210">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="211">
       <c t="s" r="A211">
         <v>328</v>
       </c>
       <c t="s" r="B211">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c t="s" r="C211">
         <v>16</v>
@@ -5215,10 +5849,13 @@
         <v>30000.0</v>
       </c>
       <c t="s" r="E211">
-        <v>358</v>
-      </c>
-    </row>
-    <row spans="1:6" r="212">
+        <v>359</v>
+      </c>
+      <c t="s" r="F211">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="212">
       <c t="s" r="A212">
         <v>328</v>
       </c>
@@ -5232,15 +5869,18 @@
         <v>220000.0</v>
       </c>
       <c t="s" r="E212">
-        <v>358</v>
-      </c>
-    </row>
-    <row spans="1:6" r="213">
+        <v>359</v>
+      </c>
+      <c t="s" r="F212">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="213">
       <c t="s" r="A213">
         <v>328</v>
       </c>
       <c t="s" r="B213">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c t="s" r="C213">
         <v>13</v>
@@ -5249,10 +5889,13 @@
         <v>380000.0</v>
       </c>
       <c t="s" r="E213">
-        <v>358</v>
-      </c>
-    </row>
-    <row spans="1:6" r="214">
+        <v>359</v>
+      </c>
+      <c t="s" r="F213">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="214">
       <c t="s" r="A214">
         <v>328</v>
       </c>
@@ -5266,10 +5909,13 @@
         <v>30000.0</v>
       </c>
       <c t="s" r="E214">
-        <v>358</v>
-      </c>
-    </row>
-    <row spans="1:6" r="215">
+        <v>359</v>
+      </c>
+      <c t="s" r="F214">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="215">
       <c t="s" r="A215">
         <v>217</v>
       </c>
@@ -5283,10 +5929,13 @@
         <v>280000.0</v>
       </c>
       <c t="s" r="E215">
-        <v>358</v>
-      </c>
-    </row>
-    <row spans="1:6" r="216">
+        <v>359</v>
+      </c>
+      <c t="s" r="F215">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="216">
       <c t="s" r="A216">
         <v>217</v>
       </c>
@@ -5300,10 +5949,13 @@
         <v>0.0</v>
       </c>
       <c t="s" r="E216">
-        <v>358</v>
-      </c>
-    </row>
-    <row spans="1:6" r="217">
+        <v>359</v>
+      </c>
+      <c t="s" r="F216">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="217">
       <c t="s" r="A217">
         <v>217</v>
       </c>
@@ -5317,10 +5969,13 @@
         <v>0.0</v>
       </c>
       <c t="s" r="E217">
-        <v>358</v>
-      </c>
-    </row>
-    <row spans="1:6" r="218">
+        <v>359</v>
+      </c>
+      <c t="s" r="F217">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="218">
       <c t="s" r="A218">
         <v>251</v>
       </c>
@@ -5334,10 +5989,13 @@
         <v>20000.0</v>
       </c>
       <c t="s" r="E218">
-        <v>358</v>
-      </c>
-    </row>
-    <row spans="1:6" r="219">
+        <v>359</v>
+      </c>
+      <c t="s" r="F218">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="219">
       <c t="s" r="A219">
         <v>251</v>
       </c>
@@ -5351,10 +6009,13 @@
         <v>20000.0</v>
       </c>
       <c t="s" r="E219">
-        <v>358</v>
-      </c>
-    </row>
-    <row spans="1:6" r="220">
+        <v>359</v>
+      </c>
+      <c t="s" r="F219">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="220">
       <c t="s" r="A220">
         <v>20</v>
       </c>
@@ -5368,10 +6029,13 @@
         <v>60000.0</v>
       </c>
       <c t="s" r="E220">
-        <v>358</v>
-      </c>
-    </row>
-    <row spans="1:6" r="221">
+        <v>359</v>
+      </c>
+      <c t="s" r="F220">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="221">
       <c t="s" r="A221">
         <v>272</v>
       </c>
@@ -5385,10 +6049,13 @@
         <v>67822.0</v>
       </c>
       <c t="s" r="E221">
-        <v>358</v>
-      </c>
-    </row>
-    <row spans="1:6" r="222">
+        <v>359</v>
+      </c>
+      <c t="s" r="F221">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="222">
       <c t="s" r="A222">
         <v>216</v>
       </c>
@@ -5402,15 +6069,18 @@
         <v>60000.0</v>
       </c>
       <c t="s" r="E222">
-        <v>358</v>
-      </c>
-    </row>
-    <row spans="1:6" r="223">
+        <v>359</v>
+      </c>
+      <c t="s" r="F222">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="223">
       <c t="s" r="A223">
         <v>142</v>
       </c>
       <c t="s" r="B223">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c t="s" r="C223">
         <v>110</v>
@@ -5419,10 +6089,13 @@
         <v>2138000.0</v>
       </c>
       <c t="s" r="E223">
-        <v>358</v>
-      </c>
-    </row>
-    <row spans="1:6" r="224">
+        <v>359</v>
+      </c>
+      <c t="s" r="F223">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="224">
       <c t="s" r="A224">
         <v>142</v>
       </c>
@@ -5436,10 +6109,13 @@
         <v>428000.0</v>
       </c>
       <c t="s" r="E224">
-        <v>358</v>
-      </c>
-    </row>
-    <row spans="1:6" r="225">
+        <v>359</v>
+      </c>
+      <c t="s" r="F224">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="225">
       <c t="s" r="A225">
         <v>142</v>
       </c>
@@ -5453,10 +6129,13 @@
         <v>560000.0</v>
       </c>
       <c t="s" r="E225">
-        <v>358</v>
-      </c>
-    </row>
-    <row spans="1:6" r="226">
+        <v>359</v>
+      </c>
+      <c t="s" r="F225">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="226">
       <c t="s" r="A226">
         <v>142</v>
       </c>
@@ -5470,15 +6149,18 @@
         <v>169000.0</v>
       </c>
       <c t="s" r="E226">
-        <v>358</v>
-      </c>
-    </row>
-    <row spans="1:6" r="227">
+        <v>359</v>
+      </c>
+      <c t="s" r="F226">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="227">
       <c t="s" r="A227">
         <v>142</v>
       </c>
       <c t="s" r="B227">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c t="s" r="C227">
         <v>110</v>
@@ -5487,15 +6169,18 @@
         <v>174000.0</v>
       </c>
       <c t="s" r="E227">
-        <v>358</v>
-      </c>
-    </row>
-    <row spans="1:6" r="228">
+        <v>359</v>
+      </c>
+      <c t="s" r="F227">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="228">
       <c t="s" r="A228">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c t="s" r="B228">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c t="s" r="C228">
         <v>62</v>
@@ -5504,12 +6189,15 @@
         <v>94500.0</v>
       </c>
       <c t="s" r="E228">
-        <v>344</v>
-      </c>
-    </row>
-    <row spans="1:6" r="229">
+        <v>345</v>
+      </c>
+      <c t="s" r="F228">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="229">
       <c t="s" r="A229">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c t="s" r="B229">
         <v>246</v>
@@ -5521,10 +6209,13 @@
         <v>447000.0</v>
       </c>
       <c t="s" r="E229">
-        <v>344</v>
-      </c>
-    </row>
-    <row spans="1:6" r="230">
+        <v>345</v>
+      </c>
+      <c t="s" r="F229">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="230">
       <c t="s" r="A230">
         <v>124</v>
       </c>
@@ -5538,10 +6229,13 @@
         <v>30000.0</v>
       </c>
       <c t="s" r="E230">
-        <v>344</v>
-      </c>
-    </row>
-    <row spans="1:6" r="231">
+        <v>345</v>
+      </c>
+      <c t="s" r="F230">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="231">
       <c t="s" r="A231">
         <v>125</v>
       </c>
@@ -5555,10 +6249,13 @@
         <v>30000.0</v>
       </c>
       <c t="s" r="E231">
-        <v>344</v>
-      </c>
-    </row>
-    <row spans="1:6" r="232">
+        <v>345</v>
+      </c>
+      <c t="s" r="F231">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="232">
       <c t="s" r="A232">
         <v>126</v>
       </c>
@@ -5572,10 +6269,13 @@
         <v>30000.0</v>
       </c>
       <c t="s" r="E232">
-        <v>344</v>
-      </c>
-    </row>
-    <row spans="1:6" r="233">
+        <v>345</v>
+      </c>
+      <c t="s" r="F232">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:7" r="233">
       <c t="s" r="A233">
         <v>286</v>
       </c>
@@ -5590,6 +6290,9 @@
       </c>
       <c t="s" r="E233">
         <v>285</v>
+      </c>
+      <c t="s" r="F233">
+        <v>350</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add parsed 農委會 result.
注意：
- 日期只有月、日是正確的，其他年時分秒都要忽略（原始格式錯誤）
- 檔名保留原樣
</commit_message>
<xml_diff>
--- a/1_政策宣傳執情形/parsed/農委會/農委會主管101年廣宣彙整.xlsx
+++ b/1_政策宣傳執情形/parsed/農委會/農委會主管101年廣宣彙整.xlsx
@@ -1613,9 +1613,9 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
-    <outlinePr summaryRight="1" summaryBelow="1"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:G233"/>
+  <dimension ref="A1:G232"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1" activeCell="A1"/>
@@ -1623,35 +1623,35 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col max="1" min="1" width="9.10"/>
-    <col max="2" min="2" width="9.10"/>
-    <col max="3" min="3" width="9.10"/>
-    <col max="4" min="4" width="9.10"/>
-    <col max="5" min="5" width="9.10"/>
-    <col max="6" min="6" width="9.10"/>
-    <col max="7" min="7" width="9.10"/>
+    <col min="1" max="1" width="9.10"/>
+    <col min="2" max="2" width="9.10"/>
+    <col min="3" max="3" width="9.10"/>
+    <col min="4" max="4" width="9.10"/>
+    <col min="5" max="5" width="9.10"/>
+    <col min="6" max="6" width="9.10"/>
+    <col min="7" max="7" width="9.10"/>
   </cols>
   <sheetData>
     <row spans="1:7" r="1">
-      <c t="s" s="1" r="A1">
+      <c s="1" t="s" r="A1">
         <v>120</v>
       </c>
-      <c t="s" s="1" r="B1">
+      <c s="1" t="s" r="B1">
         <v>209</v>
       </c>
-      <c t="s" s="1" r="C1">
+      <c s="1" t="s" r="C1">
         <v>257</v>
       </c>
-      <c t="s" s="1" r="D1">
+      <c s="1" t="s" r="D1">
         <v>361</v>
       </c>
-      <c t="s" s="1" r="E1">
+      <c s="1" t="s" r="E1">
         <v>149</v>
       </c>
-      <c t="s" s="1" r="F1">
+      <c s="1" t="s" r="F1">
         <v>333</v>
       </c>
-      <c t="s" s="1" r="G1">
+      <c s="1" t="s" r="G1">
         <v>123</v>
       </c>
     </row>
@@ -3977,7 +3977,7 @@
     </row>
     <row spans="1:7" r="118">
       <c t="s" r="A118">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c t="s" r="B118">
         <v>380</v>
@@ -3997,7 +3997,7 @@
     </row>
     <row spans="1:7" r="119">
       <c t="s" r="A119">
-        <v>270</v>
+        <v>346</v>
       </c>
       <c t="s" r="B119">
         <v>380</v>
@@ -4017,7 +4017,7 @@
     </row>
     <row spans="1:7" r="120">
       <c t="s" r="A120">
-        <v>346</v>
+        <v>135</v>
       </c>
       <c t="s" r="B120">
         <v>380</v>
@@ -4037,7 +4037,7 @@
     </row>
     <row spans="1:7" r="121">
       <c t="s" r="A121">
-        <v>135</v>
+        <v>332</v>
       </c>
       <c t="s" r="B121">
         <v>380</v>
@@ -4057,7 +4057,7 @@
     </row>
     <row spans="1:7" r="122">
       <c t="s" r="A122">
-        <v>332</v>
+        <v>25</v>
       </c>
       <c t="s" r="B122">
         <v>380</v>
@@ -4077,7 +4077,7 @@
     </row>
     <row spans="1:7" r="123">
       <c t="s" r="A123">
-        <v>25</v>
+        <v>208</v>
       </c>
       <c t="s" r="B123">
         <v>380</v>
@@ -4097,7 +4097,7 @@
     </row>
     <row spans="1:7" r="124">
       <c t="s" r="A124">
-        <v>208</v>
+        <v>280</v>
       </c>
       <c t="s" r="B124">
         <v>380</v>
@@ -4117,7 +4117,7 @@
     </row>
     <row spans="1:7" r="125">
       <c t="s" r="A125">
-        <v>280</v>
+        <v>299</v>
       </c>
       <c t="s" r="B125">
         <v>380</v>
@@ -4137,7 +4137,7 @@
     </row>
     <row spans="1:7" r="126">
       <c t="s" r="A126">
-        <v>299</v>
+        <v>116</v>
       </c>
       <c t="s" r="B126">
         <v>380</v>
@@ -4157,7 +4157,7 @@
     </row>
     <row spans="1:7" r="127">
       <c t="s" r="A127">
-        <v>116</v>
+        <v>250</v>
       </c>
       <c t="s" r="B127">
         <v>380</v>
@@ -4177,7 +4177,7 @@
     </row>
     <row spans="1:7" r="128">
       <c t="s" r="A128">
-        <v>250</v>
+        <v>398</v>
       </c>
       <c t="s" r="B128">
         <v>380</v>
@@ -4197,7 +4197,7 @@
     </row>
     <row spans="1:7" r="129">
       <c t="s" r="A129">
-        <v>398</v>
+        <v>389</v>
       </c>
       <c t="s" r="B129">
         <v>380</v>
@@ -4217,7 +4217,7 @@
     </row>
     <row spans="1:7" r="130">
       <c t="s" r="A130">
-        <v>389</v>
+        <v>335</v>
       </c>
       <c t="s" r="B130">
         <v>380</v>
@@ -4237,7 +4237,7 @@
     </row>
     <row spans="1:7" r="131">
       <c t="s" r="A131">
-        <v>335</v>
+        <v>269</v>
       </c>
       <c t="s" r="B131">
         <v>380</v>
@@ -4257,7 +4257,7 @@
     </row>
     <row spans="1:7" r="132">
       <c t="s" r="A132">
-        <v>269</v>
+        <v>320</v>
       </c>
       <c t="s" r="B132">
         <v>380</v>
@@ -4277,16 +4277,16 @@
     </row>
     <row spans="1:7" r="133">
       <c t="s" r="A133">
-        <v>320</v>
+        <v>116</v>
       </c>
       <c t="s" r="B133">
-        <v>380</v>
+        <v>181</v>
       </c>
       <c t="s" r="C133">
-        <v>40</v>
+        <v>79</v>
       </c>
       <c t="n" r="D133">
-        <v>0.0</v>
+        <v>120000.0</v>
       </c>
       <c t="s" r="E133">
         <v>276</v>
@@ -4297,16 +4297,16 @@
     </row>
     <row spans="1:7" r="134">
       <c t="s" r="A134">
-        <v>116</v>
+        <v>277</v>
       </c>
       <c t="s" r="B134">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c t="s" r="C134">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c t="n" r="D134">
-        <v>120000.0</v>
+        <v>96000.0</v>
       </c>
       <c t="s" r="E134">
         <v>276</v>
@@ -4320,13 +4320,13 @@
         <v>277</v>
       </c>
       <c t="s" r="B135">
-        <v>170</v>
+        <v>239</v>
       </c>
       <c t="s" r="C135">
         <v>87</v>
       </c>
       <c t="n" r="D135">
-        <v>96000.0</v>
+        <v>80000.0</v>
       </c>
       <c t="s" r="E135">
         <v>276</v>
@@ -4337,13 +4337,13 @@
     </row>
     <row spans="1:7" r="136">
       <c t="s" r="A136">
-        <v>277</v>
+        <v>292</v>
       </c>
       <c t="s" r="B136">
-        <v>239</v>
+        <v>338</v>
       </c>
       <c t="s" r="C136">
-        <v>87</v>
+        <v>105</v>
       </c>
       <c t="n" r="D136">
         <v>80000.0</v>
@@ -4360,13 +4360,13 @@
         <v>292</v>
       </c>
       <c t="s" r="B137">
-        <v>338</v>
+        <v>180</v>
       </c>
       <c t="s" r="C137">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c t="n" r="D137">
-        <v>80000.0</v>
+        <v>120000.0</v>
       </c>
       <c t="s" r="E137">
         <v>276</v>
@@ -4377,16 +4377,16 @@
     </row>
     <row spans="1:7" r="138">
       <c t="s" r="A138">
-        <v>292</v>
+        <v>262</v>
       </c>
       <c t="s" r="B138">
-        <v>180</v>
+        <v>340</v>
       </c>
       <c t="s" r="C138">
-        <v>103</v>
+        <v>33</v>
       </c>
       <c t="n" r="D138">
-        <v>120000.0</v>
+        <v>100000.0</v>
       </c>
       <c t="s" r="E138">
         <v>276</v>
@@ -4400,13 +4400,13 @@
         <v>262</v>
       </c>
       <c t="s" r="B139">
-        <v>340</v>
+        <v>181</v>
       </c>
       <c t="s" r="C139">
         <v>33</v>
       </c>
       <c t="n" r="D139">
-        <v>100000.0</v>
+        <v>120000.0</v>
       </c>
       <c t="s" r="E139">
         <v>276</v>
@@ -4417,7 +4417,7 @@
     </row>
     <row spans="1:7" r="140">
       <c t="s" r="A140">
-        <v>262</v>
+        <v>127</v>
       </c>
       <c t="s" r="B140">
         <v>181</v>
@@ -4440,13 +4440,13 @@
         <v>127</v>
       </c>
       <c t="s" r="B141">
-        <v>181</v>
+        <v>338</v>
       </c>
       <c t="s" r="C141">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c t="n" r="D141">
-        <v>120000.0</v>
+        <v>80000.0</v>
       </c>
       <c t="s" r="E141">
         <v>276</v>
@@ -4457,16 +4457,16 @@
     </row>
     <row spans="1:7" r="142">
       <c t="s" r="A142">
-        <v>127</v>
+        <v>291</v>
       </c>
       <c t="s" r="B142">
-        <v>338</v>
+        <v>183</v>
       </c>
       <c t="s" r="C142">
         <v>35</v>
       </c>
       <c t="n" r="D142">
-        <v>80000.0</v>
+        <v>310000.0</v>
       </c>
       <c t="s" r="E142">
         <v>276</v>
@@ -4480,13 +4480,13 @@
         <v>291</v>
       </c>
       <c t="s" r="B143">
-        <v>183</v>
+        <v>339</v>
       </c>
       <c t="s" r="C143">
         <v>35</v>
       </c>
       <c t="n" r="D143">
-        <v>310000.0</v>
+        <v>420000.0</v>
       </c>
       <c t="s" r="E143">
         <v>276</v>
@@ -4497,16 +4497,16 @@
     </row>
     <row spans="1:7" r="144">
       <c t="s" r="A144">
-        <v>291</v>
+        <v>402</v>
       </c>
       <c t="s" r="B144">
-        <v>339</v>
+        <v>183</v>
       </c>
       <c t="s" r="C144">
         <v>35</v>
       </c>
       <c t="n" r="D144">
-        <v>420000.0</v>
+        <v>200000.0</v>
       </c>
       <c t="s" r="E144">
         <v>276</v>
@@ -4520,13 +4520,13 @@
         <v>402</v>
       </c>
       <c t="s" r="B145">
-        <v>183</v>
+        <v>338</v>
       </c>
       <c t="s" r="C145">
         <v>35</v>
       </c>
       <c t="n" r="D145">
-        <v>200000.0</v>
+        <v>100000.0</v>
       </c>
       <c t="s" r="E145">
         <v>276</v>
@@ -4537,16 +4537,16 @@
     </row>
     <row spans="1:7" r="146">
       <c t="s" r="A146">
-        <v>402</v>
+        <v>281</v>
       </c>
       <c t="s" r="B146">
-        <v>338</v>
+        <v>184</v>
       </c>
       <c t="s" r="C146">
         <v>35</v>
       </c>
       <c t="n" r="D146">
-        <v>100000.0</v>
+        <v>300000.0</v>
       </c>
       <c t="s" r="E146">
         <v>276</v>
@@ -4560,13 +4560,13 @@
         <v>281</v>
       </c>
       <c t="s" r="B147">
-        <v>184</v>
+        <v>338</v>
       </c>
       <c t="s" r="C147">
         <v>35</v>
       </c>
       <c t="n" r="D147">
-        <v>300000.0</v>
+        <v>100000.0</v>
       </c>
       <c t="s" r="E147">
         <v>276</v>
@@ -4577,16 +4577,16 @@
     </row>
     <row spans="1:7" r="148">
       <c t="s" r="A148">
-        <v>281</v>
+        <v>401</v>
       </c>
       <c t="s" r="B148">
-        <v>338</v>
+        <v>379</v>
       </c>
       <c t="s" r="C148">
-        <v>35</v>
+        <v>77</v>
       </c>
       <c t="n" r="D148">
-        <v>100000.0</v>
+        <v>72000.0</v>
       </c>
       <c t="s" r="E148">
         <v>276</v>
@@ -4597,16 +4597,16 @@
     </row>
     <row spans="1:7" r="149">
       <c t="s" r="A149">
-        <v>401</v>
+        <v>210</v>
       </c>
       <c t="s" r="B149">
-        <v>379</v>
+        <v>385</v>
       </c>
       <c t="s" r="C149">
-        <v>77</v>
+        <v>34</v>
       </c>
       <c t="n" r="D149">
-        <v>72000.0</v>
+        <v>280000.0</v>
       </c>
       <c t="s" r="E149">
         <v>276</v>
@@ -4617,16 +4617,16 @@
     </row>
     <row spans="1:7" r="150">
       <c t="s" r="A150">
-        <v>210</v>
+        <v>274</v>
       </c>
       <c t="s" r="B150">
-        <v>385</v>
+        <v>275</v>
       </c>
       <c t="s" r="C150">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c t="n" r="D150">
-        <v>280000.0</v>
+        <v>3945000.0</v>
       </c>
       <c t="s" r="E150">
         <v>276</v>
@@ -4637,16 +4637,16 @@
     </row>
     <row spans="1:7" r="151">
       <c t="s" r="A151">
-        <v>274</v>
+        <v>287</v>
       </c>
       <c t="s" r="B151">
-        <v>275</v>
+        <v>379</v>
       </c>
       <c t="s" r="C151">
-        <v>40</v>
+        <v>69</v>
       </c>
       <c t="n" r="D151">
-        <v>3945000.0</v>
+        <v>95080.0</v>
       </c>
       <c t="s" r="E151">
         <v>276</v>
@@ -4657,19 +4657,19 @@
     </row>
     <row spans="1:7" r="152">
       <c t="s" r="A152">
-        <v>287</v>
+        <v>131</v>
       </c>
       <c t="s" r="B152">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c t="s" r="C152">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c t="n" r="D152">
-        <v>95080.0</v>
+        <v>40000.0</v>
       </c>
       <c t="s" r="E152">
-        <v>276</v>
+        <v>344</v>
       </c>
       <c t="s" r="F152">
         <v>350</v>
@@ -4677,19 +4677,19 @@
     </row>
     <row spans="1:7" r="153">
       <c t="s" r="A153">
-        <v>131</v>
+        <v>253</v>
       </c>
       <c t="s" r="B153">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c t="s" r="C153">
-        <v>67</v>
+        <v>2</v>
       </c>
       <c t="n" r="D153">
-        <v>40000.0</v>
+        <v>484800.0</v>
       </c>
       <c t="s" r="E153">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c t="s" r="F153">
         <v>350</v>
@@ -4697,16 +4697,16 @@
     </row>
     <row spans="1:7" r="154">
       <c t="s" r="A154">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c t="s" r="B154">
-        <v>367</v>
+        <v>202</v>
       </c>
       <c t="s" r="C154">
         <v>2</v>
       </c>
       <c t="n" r="D154">
-        <v>484800.0</v>
+        <v>1400000.0</v>
       </c>
       <c t="s" r="E154">
         <v>343</v>
@@ -4717,16 +4717,16 @@
     </row>
     <row spans="1:7" r="155">
       <c t="s" r="A155">
-        <v>254</v>
+        <v>341</v>
       </c>
       <c t="s" r="B155">
-        <v>202</v>
+        <v>375</v>
       </c>
       <c t="s" r="C155">
-        <v>2</v>
+        <v>53</v>
       </c>
       <c t="n" r="D155">
-        <v>1400000.0</v>
+        <v>320000.0</v>
       </c>
       <c t="s" r="E155">
         <v>343</v>
@@ -4737,16 +4737,16 @@
     </row>
     <row spans="1:7" r="156">
       <c t="s" r="A156">
-        <v>341</v>
+        <v>283</v>
       </c>
       <c t="s" r="B156">
-        <v>375</v>
+        <v>379</v>
       </c>
       <c t="s" r="C156">
-        <v>53</v>
+        <v>80</v>
       </c>
       <c t="n" r="D156">
-        <v>320000.0</v>
+        <v>96000.0</v>
       </c>
       <c t="s" r="E156">
         <v>343</v>
@@ -4757,16 +4757,16 @@
     </row>
     <row spans="1:7" r="157">
       <c t="s" r="A157">
-        <v>283</v>
+        <v>296</v>
       </c>
       <c t="s" r="B157">
-        <v>379</v>
+        <v>387</v>
       </c>
       <c t="s" r="C157">
-        <v>80</v>
+        <v>109</v>
       </c>
       <c t="n" r="D157">
-        <v>96000.0</v>
+        <v>2171000.0</v>
       </c>
       <c t="s" r="E157">
         <v>343</v>
@@ -4780,13 +4780,13 @@
         <v>296</v>
       </c>
       <c t="s" r="B158">
-        <v>387</v>
+        <v>302</v>
       </c>
       <c t="s" r="C158">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c t="n" r="D158">
-        <v>2171000.0</v>
+        <v>600000.0</v>
       </c>
       <c t="s" r="E158">
         <v>343</v>
@@ -4797,16 +4797,16 @@
     </row>
     <row spans="1:7" r="159">
       <c t="s" r="A159">
-        <v>296</v>
+        <v>130</v>
       </c>
       <c t="s" r="B159">
-        <v>302</v>
+        <v>203</v>
       </c>
       <c t="s" r="C159">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c t="n" r="D159">
-        <v>600000.0</v>
+        <v>820600.0</v>
       </c>
       <c t="s" r="E159">
         <v>343</v>
@@ -4820,13 +4820,13 @@
         <v>130</v>
       </c>
       <c t="s" r="B160">
-        <v>203</v>
+        <v>303</v>
       </c>
       <c t="s" r="C160">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c t="n" r="D160">
-        <v>820600.0</v>
+        <v>105000.0</v>
       </c>
       <c t="s" r="E160">
         <v>343</v>
@@ -4837,16 +4837,16 @@
     </row>
     <row spans="1:7" r="161">
       <c t="s" r="A161">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c t="s" r="B161">
-        <v>303</v>
+        <v>379</v>
       </c>
       <c t="s" r="C161">
-        <v>102</v>
+        <v>34</v>
       </c>
       <c t="n" r="D161">
-        <v>105000.0</v>
+        <v>50400.0</v>
       </c>
       <c t="s" r="E161">
         <v>343</v>
@@ -4857,16 +4857,16 @@
     </row>
     <row spans="1:7" r="162">
       <c t="s" r="A162">
-        <v>115</v>
+        <v>290</v>
       </c>
       <c t="s" r="B162">
         <v>379</v>
       </c>
       <c t="s" r="C162">
-        <v>34</v>
+        <v>84</v>
       </c>
       <c t="n" r="D162">
-        <v>50400.0</v>
+        <v>95000.0</v>
       </c>
       <c t="s" r="E162">
         <v>343</v>
@@ -4877,16 +4877,16 @@
     </row>
     <row spans="1:7" r="163">
       <c t="s" r="A163">
-        <v>290</v>
+        <v>298</v>
       </c>
       <c t="s" r="B163">
         <v>379</v>
       </c>
       <c t="s" r="C163">
-        <v>84</v>
+        <v>35</v>
       </c>
       <c t="n" r="D163">
-        <v>95000.0</v>
+        <v>50000.0</v>
       </c>
       <c t="s" r="E163">
         <v>343</v>
@@ -4897,16 +4897,16 @@
     </row>
     <row spans="1:7" r="164">
       <c t="s" r="A164">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c t="s" r="B164">
-        <v>379</v>
+        <v>191</v>
       </c>
       <c t="s" r="C164">
         <v>35</v>
       </c>
       <c t="n" r="D164">
-        <v>50000.0</v>
+        <v>208500.0</v>
       </c>
       <c t="s" r="E164">
         <v>343</v>
@@ -4917,16 +4917,16 @@
     </row>
     <row spans="1:7" r="165">
       <c t="s" r="A165">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c t="s" r="B165">
-        <v>191</v>
+        <v>374</v>
       </c>
       <c t="s" r="C165">
         <v>35</v>
       </c>
       <c t="n" r="D165">
-        <v>208500.0</v>
+        <v>90000.0</v>
       </c>
       <c t="s" r="E165">
         <v>343</v>
@@ -4940,13 +4940,13 @@
         <v>289</v>
       </c>
       <c t="s" r="B166">
-        <v>374</v>
+        <v>302</v>
       </c>
       <c t="s" r="C166">
         <v>35</v>
       </c>
       <c t="n" r="D166">
-        <v>90000.0</v>
+        <v>81000.0</v>
       </c>
       <c t="s" r="E166">
         <v>343</v>
@@ -4957,19 +4957,19 @@
     </row>
     <row spans="1:7" r="167">
       <c t="s" r="A167">
-        <v>289</v>
+        <v>116</v>
       </c>
       <c t="s" r="B167">
-        <v>302</v>
+        <v>155</v>
       </c>
       <c t="s" r="C167">
-        <v>35</v>
+        <v>79</v>
       </c>
       <c t="n" r="D167">
-        <v>81000.0</v>
+        <v>508800.0</v>
       </c>
       <c t="s" r="E167">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c t="s" r="F167">
         <v>350</v>
@@ -4977,16 +4977,16 @@
     </row>
     <row spans="1:7" r="168">
       <c t="s" r="A168">
-        <v>116</v>
+        <v>292</v>
       </c>
       <c t="s" r="B168">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c t="s" r="C168">
-        <v>79</v>
+        <v>103</v>
       </c>
       <c t="n" r="D168">
-        <v>508800.0</v>
+        <v>351000.0</v>
       </c>
       <c t="s" r="E168">
         <v>342</v>
@@ -4997,16 +4997,16 @@
     </row>
     <row spans="1:7" r="169">
       <c t="s" r="A169">
-        <v>292</v>
+        <v>127</v>
       </c>
       <c t="s" r="B169">
-        <v>154</v>
+        <v>193</v>
       </c>
       <c t="s" r="C169">
-        <v>103</v>
+        <v>33</v>
       </c>
       <c t="n" r="D169">
-        <v>351000.0</v>
+        <v>175500.0</v>
       </c>
       <c t="s" r="E169">
         <v>342</v>
@@ -5017,16 +5017,16 @@
     </row>
     <row spans="1:7" r="170">
       <c t="s" r="A170">
-        <v>127</v>
+        <v>262</v>
       </c>
       <c t="s" r="B170">
-        <v>193</v>
+        <v>155</v>
       </c>
       <c t="s" r="C170">
         <v>33</v>
       </c>
       <c t="n" r="D170">
-        <v>175500.0</v>
+        <v>292500.0</v>
       </c>
       <c t="s" r="E170">
         <v>342</v>
@@ -5037,19 +5037,19 @@
     </row>
     <row spans="1:7" r="171">
       <c t="s" r="A171">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c t="s" r="B171">
-        <v>155</v>
+        <v>390</v>
       </c>
       <c t="s" r="C171">
-        <v>33</v>
+        <v>71</v>
       </c>
       <c t="n" r="D171">
-        <v>292500.0</v>
+        <v>17000.0</v>
       </c>
       <c t="s" r="E171">
-        <v>342</v>
+        <v>264</v>
       </c>
       <c t="s" r="F171">
         <v>350</v>
@@ -5060,13 +5060,13 @@
         <v>266</v>
       </c>
       <c t="s" r="B172">
-        <v>390</v>
+        <v>308</v>
       </c>
       <c t="s" r="C172">
         <v>71</v>
       </c>
       <c t="n" r="D172">
-        <v>17000.0</v>
+        <v>6000.0</v>
       </c>
       <c t="s" r="E172">
         <v>264</v>
@@ -5080,13 +5080,13 @@
         <v>266</v>
       </c>
       <c t="s" r="B173">
-        <v>308</v>
+        <v>236</v>
       </c>
       <c t="s" r="C173">
         <v>71</v>
       </c>
       <c t="n" r="D173">
-        <v>6000.0</v>
+        <v>15000.0</v>
       </c>
       <c t="s" r="E173">
         <v>264</v>
@@ -5097,16 +5097,16 @@
     </row>
     <row spans="1:7" r="174">
       <c t="s" r="A174">
-        <v>266</v>
+        <v>147</v>
       </c>
       <c t="s" r="B174">
-        <v>236</v>
+        <v>390</v>
       </c>
       <c t="s" r="C174">
         <v>71</v>
       </c>
       <c t="n" r="D174">
-        <v>15000.0</v>
+        <v>91500.0</v>
       </c>
       <c t="s" r="E174">
         <v>264</v>
@@ -5120,13 +5120,13 @@
         <v>147</v>
       </c>
       <c t="s" r="B175">
-        <v>390</v>
+        <v>308</v>
       </c>
       <c t="s" r="C175">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c t="n" r="D175">
-        <v>91500.0</v>
+        <v>15000.0</v>
       </c>
       <c t="s" r="E175">
         <v>264</v>
@@ -5140,13 +5140,13 @@
         <v>147</v>
       </c>
       <c t="s" r="B176">
-        <v>308</v>
+        <v>177</v>
       </c>
       <c t="s" r="C176">
         <v>82</v>
       </c>
       <c t="n" r="D176">
-        <v>15000.0</v>
+        <v>446220.0</v>
       </c>
       <c t="s" r="E176">
         <v>264</v>
@@ -5160,13 +5160,13 @@
         <v>147</v>
       </c>
       <c t="s" r="B177">
-        <v>177</v>
+        <v>231</v>
       </c>
       <c t="s" r="C177">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c t="n" r="D177">
-        <v>446220.0</v>
+        <v>122111.0</v>
       </c>
       <c t="s" r="E177">
         <v>264</v>
@@ -5177,16 +5177,16 @@
     </row>
     <row spans="1:7" r="178">
       <c t="s" r="A178">
-        <v>147</v>
+        <v>288</v>
       </c>
       <c t="s" r="B178">
-        <v>231</v>
+        <v>390</v>
       </c>
       <c t="s" r="C178">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c t="n" r="D178">
-        <v>122111.0</v>
+        <v>17000.0</v>
       </c>
       <c t="s" r="E178">
         <v>264</v>
@@ -5200,13 +5200,13 @@
         <v>288</v>
       </c>
       <c t="s" r="B179">
-        <v>390</v>
+        <v>308</v>
       </c>
       <c t="s" r="C179">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c t="n" r="D179">
-        <v>17000.0</v>
+        <v>15000.0</v>
       </c>
       <c t="s" r="E179">
         <v>264</v>
@@ -5220,10 +5220,10 @@
         <v>288</v>
       </c>
       <c t="s" r="B180">
-        <v>308</v>
+        <v>167</v>
       </c>
       <c t="s" r="C180">
-        <v>79</v>
+        <v>35</v>
       </c>
       <c t="n" r="D180">
         <v>15000.0</v>
@@ -5240,13 +5240,13 @@
         <v>288</v>
       </c>
       <c t="s" r="B181">
-        <v>167</v>
+        <v>230</v>
       </c>
       <c t="s" r="C181">
-        <v>35</v>
+        <v>79</v>
       </c>
       <c t="n" r="D181">
-        <v>15000.0</v>
+        <v>24917.0</v>
       </c>
       <c t="s" r="E181">
         <v>264</v>
@@ -5257,16 +5257,16 @@
     </row>
     <row spans="1:7" r="182">
       <c t="s" r="A182">
-        <v>288</v>
+        <v>22</v>
       </c>
       <c t="s" r="B182">
-        <v>230</v>
+        <v>377</v>
       </c>
       <c t="s" r="C182">
-        <v>79</v>
+        <v>35</v>
       </c>
       <c t="n" r="D182">
-        <v>24917.0</v>
+        <v>29166.0</v>
       </c>
       <c t="s" r="E182">
         <v>264</v>
@@ -5280,13 +5280,13 @@
         <v>22</v>
       </c>
       <c t="s" r="B183">
-        <v>377</v>
+        <v>240</v>
       </c>
       <c t="s" r="C183">
-        <v>35</v>
+        <v>89</v>
       </c>
       <c t="n" r="D183">
-        <v>29166.0</v>
+        <v>131251.0</v>
       </c>
       <c t="s" r="E183">
         <v>264</v>
@@ -5297,16 +5297,16 @@
     </row>
     <row spans="1:7" r="184">
       <c t="s" r="A184">
-        <v>22</v>
+        <v>297</v>
       </c>
       <c t="s" r="B184">
         <v>240</v>
       </c>
       <c t="s" r="C184">
-        <v>89</v>
+        <v>72</v>
       </c>
       <c t="n" r="D184">
-        <v>131251.0</v>
+        <v>61251.0</v>
       </c>
       <c t="s" r="E184">
         <v>264</v>
@@ -5320,13 +5320,13 @@
         <v>297</v>
       </c>
       <c t="s" r="B185">
-        <v>240</v>
+        <v>179</v>
       </c>
       <c t="s" r="C185">
-        <v>72</v>
+        <v>107</v>
       </c>
       <c t="n" r="D185">
-        <v>61251.0</v>
+        <v>323603.0</v>
       </c>
       <c t="s" r="E185">
         <v>264</v>
@@ -5337,16 +5337,16 @@
     </row>
     <row spans="1:7" r="186">
       <c t="s" r="A186">
-        <v>297</v>
+        <v>265</v>
       </c>
       <c t="s" r="B186">
-        <v>179</v>
+        <v>242</v>
       </c>
       <c t="s" r="C186">
-        <v>107</v>
+        <v>81</v>
       </c>
       <c t="n" r="D186">
-        <v>323603.0</v>
+        <v>23819.0</v>
       </c>
       <c t="s" r="E186">
         <v>264</v>
@@ -5360,13 +5360,13 @@
         <v>265</v>
       </c>
       <c t="s" r="B187">
-        <v>242</v>
+        <v>194</v>
       </c>
       <c t="s" r="C187">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c t="n" r="D187">
-        <v>23819.0</v>
+        <v>15000.0</v>
       </c>
       <c t="s" r="E187">
         <v>264</v>
@@ -5377,16 +5377,16 @@
     </row>
     <row spans="1:7" r="188">
       <c t="s" r="A188">
-        <v>265</v>
+        <v>148</v>
       </c>
       <c t="s" r="B188">
-        <v>194</v>
+        <v>153</v>
       </c>
       <c t="s" r="C188">
-        <v>79</v>
+        <v>35</v>
       </c>
       <c t="n" r="D188">
-        <v>15000.0</v>
+        <v>380000.0</v>
       </c>
       <c t="s" r="E188">
         <v>264</v>
@@ -5400,13 +5400,13 @@
         <v>148</v>
       </c>
       <c t="s" r="B189">
-        <v>153</v>
+        <v>230</v>
       </c>
       <c t="s" r="C189">
-        <v>35</v>
+        <v>82</v>
       </c>
       <c t="n" r="D189">
-        <v>380000.0</v>
+        <v>30617.0</v>
       </c>
       <c t="s" r="E189">
         <v>264</v>
@@ -5417,16 +5417,16 @@
     </row>
     <row spans="1:7" r="190">
       <c t="s" r="A190">
-        <v>148</v>
+        <v>353</v>
       </c>
       <c t="s" r="B190">
-        <v>230</v>
+        <v>309</v>
       </c>
       <c t="s" r="C190">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c t="n" r="D190">
-        <v>30617.0</v>
+        <v>105000.0</v>
       </c>
       <c t="s" r="E190">
         <v>264</v>
@@ -5440,13 +5440,13 @@
         <v>353</v>
       </c>
       <c t="s" r="B191">
-        <v>309</v>
+        <v>192</v>
       </c>
       <c t="s" r="C191">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c t="n" r="D191">
-        <v>105000.0</v>
+        <v>900000.0</v>
       </c>
       <c t="s" r="E191">
         <v>264</v>
@@ -5460,13 +5460,13 @@
         <v>353</v>
       </c>
       <c t="s" r="B192">
-        <v>192</v>
+        <v>241</v>
       </c>
       <c t="s" r="C192">
-        <v>87</v>
+        <v>70</v>
       </c>
       <c t="n" r="D192">
-        <v>900000.0</v>
+        <v>129702.0</v>
       </c>
       <c t="s" r="E192">
         <v>264</v>
@@ -5477,16 +5477,16 @@
     </row>
     <row spans="1:7" r="193">
       <c t="s" r="A193">
-        <v>353</v>
+        <v>114</v>
       </c>
       <c t="s" r="B193">
-        <v>241</v>
+        <v>390</v>
       </c>
       <c t="s" r="C193">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c t="n" r="D193">
-        <v>129702.0</v>
+        <v>8500.0</v>
       </c>
       <c t="s" r="E193">
         <v>264</v>
@@ -5500,13 +5500,13 @@
         <v>114</v>
       </c>
       <c t="s" r="B194">
-        <v>390</v>
+        <v>308</v>
       </c>
       <c t="s" r="C194">
         <v>87</v>
       </c>
       <c t="n" r="D194">
-        <v>8500.0</v>
+        <v>3000.0</v>
       </c>
       <c t="s" r="E194">
         <v>264</v>
@@ -5520,13 +5520,13 @@
         <v>114</v>
       </c>
       <c t="s" r="B195">
-        <v>308</v>
+        <v>167</v>
       </c>
       <c t="s" r="C195">
         <v>87</v>
       </c>
       <c t="n" r="D195">
-        <v>3000.0</v>
+        <v>15000.0</v>
       </c>
       <c t="s" r="E195">
         <v>264</v>
@@ -5540,13 +5540,13 @@
         <v>114</v>
       </c>
       <c t="s" r="B196">
-        <v>167</v>
+        <v>240</v>
       </c>
       <c t="s" r="C196">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c t="n" r="D196">
-        <v>15000.0</v>
+        <v>20417.0</v>
       </c>
       <c t="s" r="E196">
         <v>264</v>
@@ -5557,16 +5557,16 @@
     </row>
     <row spans="1:7" r="197">
       <c t="s" r="A197">
-        <v>114</v>
+        <v>267</v>
       </c>
       <c t="s" r="B197">
-        <v>240</v>
+        <v>369</v>
       </c>
       <c t="s" r="C197">
-        <v>97</v>
+        <v>35</v>
       </c>
       <c t="n" r="D197">
-        <v>20417.0</v>
+        <v>90000.0</v>
       </c>
       <c t="s" r="E197">
         <v>264</v>
@@ -5580,13 +5580,13 @@
         <v>267</v>
       </c>
       <c t="s" r="B198">
-        <v>369</v>
+        <v>232</v>
       </c>
       <c t="s" r="C198">
-        <v>35</v>
+        <v>106</v>
       </c>
       <c t="n" r="D198">
-        <v>90000.0</v>
+        <v>200000.0</v>
       </c>
       <c t="s" r="E198">
         <v>264</v>
@@ -5597,16 +5597,16 @@
     </row>
     <row spans="1:7" r="199">
       <c t="s" r="A199">
-        <v>267</v>
+        <v>334</v>
       </c>
       <c t="s" r="B199">
-        <v>232</v>
+        <v>240</v>
       </c>
       <c t="s" r="C199">
-        <v>106</v>
+        <v>33</v>
       </c>
       <c t="n" r="D199">
-        <v>200000.0</v>
+        <v>20417.0</v>
       </c>
       <c t="s" r="E199">
         <v>264</v>
@@ -5617,16 +5617,16 @@
     </row>
     <row spans="1:7" r="200">
       <c t="s" r="A200">
-        <v>334</v>
+        <v>26</v>
       </c>
       <c t="s" r="B200">
-        <v>240</v>
+        <v>190</v>
       </c>
       <c t="s" r="C200">
         <v>33</v>
       </c>
       <c t="n" r="D200">
-        <v>20417.0</v>
+        <v>380000.0</v>
       </c>
       <c t="s" r="E200">
         <v>264</v>
@@ -5640,13 +5640,13 @@
         <v>26</v>
       </c>
       <c t="s" r="B201">
-        <v>190</v>
+        <v>240</v>
       </c>
       <c t="s" r="C201">
-        <v>33</v>
+        <v>98</v>
       </c>
       <c t="n" r="D201">
-        <v>380000.0</v>
+        <v>40834.0</v>
       </c>
       <c t="s" r="E201">
         <v>264</v>
@@ -5657,16 +5657,16 @@
     </row>
     <row spans="1:7" r="202">
       <c t="s" r="A202">
-        <v>26</v>
+        <v>352</v>
       </c>
       <c t="s" r="B202">
-        <v>240</v>
+        <v>174</v>
       </c>
       <c t="s" r="C202">
-        <v>98</v>
+        <v>33</v>
       </c>
       <c t="n" r="D202">
-        <v>40834.0</v>
+        <v>0.0</v>
       </c>
       <c t="s" r="E202">
         <v>264</v>
@@ -5680,13 +5680,13 @@
         <v>352</v>
       </c>
       <c t="s" r="B203">
-        <v>174</v>
+        <v>240</v>
       </c>
       <c t="s" r="C203">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c t="n" r="D203">
-        <v>0.0</v>
+        <v>20417.0</v>
       </c>
       <c t="s" r="E203">
         <v>264</v>
@@ -5697,19 +5697,19 @@
     </row>
     <row spans="1:7" r="204">
       <c t="s" r="A204">
-        <v>352</v>
+        <v>212</v>
       </c>
       <c t="s" r="B204">
-        <v>240</v>
+        <v>314</v>
       </c>
       <c t="s" r="C204">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c t="n" r="D204">
-        <v>20417.0</v>
+        <v>60000.0</v>
       </c>
       <c t="s" r="E204">
-        <v>264</v>
+        <v>359</v>
       </c>
       <c t="s" r="F204">
         <v>350</v>
@@ -5717,16 +5717,16 @@
     </row>
     <row spans="1:7" r="205">
       <c t="s" r="A205">
-        <v>212</v>
+        <v>355</v>
       </c>
       <c t="s" r="B205">
-        <v>314</v>
+        <v>263</v>
       </c>
       <c t="s" r="C205">
         <v>40</v>
       </c>
       <c t="n" r="D205">
-        <v>60000.0</v>
+        <v>2470000.0</v>
       </c>
       <c t="s" r="E205">
         <v>359</v>
@@ -5737,16 +5737,16 @@
     </row>
     <row spans="1:7" r="206">
       <c t="s" r="A206">
-        <v>355</v>
+        <v>128</v>
       </c>
       <c t="s" r="B206">
-        <v>263</v>
+        <v>119</v>
       </c>
       <c t="s" r="C206">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c t="n" r="D206">
-        <v>2470000.0</v>
+        <v>96000.0</v>
       </c>
       <c t="s" r="E206">
         <v>359</v>
@@ -5757,16 +5757,16 @@
     </row>
     <row spans="1:7" r="207">
       <c t="s" r="A207">
-        <v>128</v>
+        <v>300</v>
       </c>
       <c t="s" r="B207">
-        <v>119</v>
+        <v>360</v>
       </c>
       <c t="s" r="C207">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c t="n" r="D207">
-        <v>96000.0</v>
+        <v>88000.0</v>
       </c>
       <c t="s" r="E207">
         <v>359</v>
@@ -5777,16 +5777,16 @@
     </row>
     <row spans="1:7" r="208">
       <c t="s" r="A208">
-        <v>300</v>
+        <v>328</v>
       </c>
       <c t="s" r="B208">
-        <v>360</v>
+        <v>207</v>
       </c>
       <c t="s" r="C208">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c t="n" r="D208">
-        <v>88000.0</v>
+        <v>850000.0</v>
       </c>
       <c t="s" r="E208">
         <v>359</v>
@@ -5800,13 +5800,13 @@
         <v>328</v>
       </c>
       <c t="s" r="B209">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c t="s" r="C209">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c t="n" r="D209">
-        <v>850000.0</v>
+        <v>190000.0</v>
       </c>
       <c t="s" r="E209">
         <v>359</v>
@@ -5820,13 +5820,13 @@
         <v>328</v>
       </c>
       <c t="s" r="B210">
-        <v>206</v>
+        <v>388</v>
       </c>
       <c t="s" r="C210">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c t="n" r="D210">
-        <v>190000.0</v>
+        <v>30000.0</v>
       </c>
       <c t="s" r="E210">
         <v>359</v>
@@ -5840,13 +5840,13 @@
         <v>328</v>
       </c>
       <c t="s" r="B211">
-        <v>388</v>
+        <v>234</v>
       </c>
       <c t="s" r="C211">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c t="n" r="D211">
-        <v>30000.0</v>
+        <v>220000.0</v>
       </c>
       <c t="s" r="E211">
         <v>359</v>
@@ -5860,13 +5860,13 @@
         <v>328</v>
       </c>
       <c t="s" r="B212">
-        <v>234</v>
+        <v>394</v>
       </c>
       <c t="s" r="C212">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c t="n" r="D212">
-        <v>220000.0</v>
+        <v>380000.0</v>
       </c>
       <c t="s" r="E212">
         <v>359</v>
@@ -5880,13 +5880,13 @@
         <v>328</v>
       </c>
       <c t="s" r="B213">
-        <v>394</v>
+        <v>303</v>
       </c>
       <c t="s" r="C213">
         <v>13</v>
       </c>
       <c t="n" r="D213">
-        <v>380000.0</v>
+        <v>30000.0</v>
       </c>
       <c t="s" r="E213">
         <v>359</v>
@@ -5897,16 +5897,16 @@
     </row>
     <row spans="1:7" r="214">
       <c t="s" r="A214">
-        <v>328</v>
+        <v>217</v>
       </c>
       <c t="s" r="B214">
-        <v>303</v>
+        <v>323</v>
       </c>
       <c t="s" r="C214">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c t="n" r="D214">
-        <v>30000.0</v>
+        <v>280000.0</v>
       </c>
       <c t="s" r="E214">
         <v>359</v>
@@ -5920,13 +5920,13 @@
         <v>217</v>
       </c>
       <c t="s" r="B215">
-        <v>323</v>
+        <v>247</v>
       </c>
       <c t="s" r="C215">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c t="n" r="D215">
-        <v>280000.0</v>
+        <v>0.0</v>
       </c>
       <c t="s" r="E215">
         <v>359</v>
@@ -5940,7 +5940,7 @@
         <v>217</v>
       </c>
       <c t="s" r="B216">
-        <v>247</v>
+        <v>293</v>
       </c>
       <c t="s" r="C216">
         <v>17</v>
@@ -5957,16 +5957,16 @@
     </row>
     <row spans="1:7" r="217">
       <c t="s" r="A217">
-        <v>217</v>
+        <v>251</v>
       </c>
       <c t="s" r="B217">
-        <v>293</v>
+        <v>29</v>
       </c>
       <c t="s" r="C217">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c t="n" r="D217">
-        <v>0.0</v>
+        <v>20000.0</v>
       </c>
       <c t="s" r="E217">
         <v>359</v>
@@ -5980,10 +5980,10 @@
         <v>251</v>
       </c>
       <c t="s" r="B218">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c t="s" r="C218">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c t="n" r="D218">
         <v>20000.0</v>
@@ -5997,16 +5997,16 @@
     </row>
     <row spans="1:7" r="219">
       <c t="s" r="A219">
-        <v>251</v>
+        <v>20</v>
       </c>
       <c t="s" r="B219">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c t="s" r="C219">
-        <v>19</v>
+        <v>87</v>
       </c>
       <c t="n" r="D219">
-        <v>20000.0</v>
+        <v>60000.0</v>
       </c>
       <c t="s" r="E219">
         <v>359</v>
@@ -6017,16 +6017,16 @@
     </row>
     <row spans="1:7" r="220">
       <c t="s" r="A220">
-        <v>20</v>
+        <v>272</v>
       </c>
       <c t="s" r="B220">
-        <v>56</v>
+        <v>117</v>
       </c>
       <c t="s" r="C220">
-        <v>87</v>
+        <v>35</v>
       </c>
       <c t="n" r="D220">
-        <v>60000.0</v>
+        <v>67822.0</v>
       </c>
       <c t="s" r="E220">
         <v>359</v>
@@ -6037,16 +6037,16 @@
     </row>
     <row spans="1:7" r="221">
       <c t="s" r="A221">
-        <v>272</v>
+        <v>216</v>
       </c>
       <c t="s" r="B221">
-        <v>117</v>
+        <v>152</v>
       </c>
       <c t="s" r="C221">
         <v>35</v>
       </c>
       <c t="n" r="D221">
-        <v>67822.0</v>
+        <v>60000.0</v>
       </c>
       <c t="s" r="E221">
         <v>359</v>
@@ -6057,16 +6057,16 @@
     </row>
     <row spans="1:7" r="222">
       <c t="s" r="A222">
-        <v>216</v>
+        <v>142</v>
       </c>
       <c t="s" r="B222">
-        <v>152</v>
+        <v>396</v>
       </c>
       <c t="s" r="C222">
-        <v>35</v>
+        <v>110</v>
       </c>
       <c t="n" r="D222">
-        <v>60000.0</v>
+        <v>2138000.0</v>
       </c>
       <c t="s" r="E222">
         <v>359</v>
@@ -6080,13 +6080,13 @@
         <v>142</v>
       </c>
       <c t="s" r="B223">
-        <v>396</v>
+        <v>199</v>
       </c>
       <c t="s" r="C223">
         <v>110</v>
       </c>
       <c t="n" r="D223">
-        <v>2138000.0</v>
+        <v>428000.0</v>
       </c>
       <c t="s" r="E223">
         <v>359</v>
@@ -6100,13 +6100,13 @@
         <v>142</v>
       </c>
       <c t="s" r="B224">
-        <v>199</v>
+        <v>225</v>
       </c>
       <c t="s" r="C224">
         <v>110</v>
       </c>
       <c t="n" r="D224">
-        <v>428000.0</v>
+        <v>560000.0</v>
       </c>
       <c t="s" r="E224">
         <v>359</v>
@@ -6120,13 +6120,13 @@
         <v>142</v>
       </c>
       <c t="s" r="B225">
-        <v>225</v>
+        <v>303</v>
       </c>
       <c t="s" r="C225">
         <v>110</v>
       </c>
       <c t="n" r="D225">
-        <v>560000.0</v>
+        <v>169000.0</v>
       </c>
       <c t="s" r="E225">
         <v>359</v>
@@ -6140,13 +6140,13 @@
         <v>142</v>
       </c>
       <c t="s" r="B226">
-        <v>303</v>
+        <v>363</v>
       </c>
       <c t="s" r="C226">
         <v>110</v>
       </c>
       <c t="n" r="D226">
-        <v>169000.0</v>
+        <v>174000.0</v>
       </c>
       <c t="s" r="E226">
         <v>359</v>
@@ -6157,19 +6157,19 @@
     </row>
     <row spans="1:7" r="227">
       <c t="s" r="A227">
-        <v>142</v>
+        <v>348</v>
       </c>
       <c t="s" r="B227">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c t="s" r="C227">
-        <v>110</v>
+        <v>62</v>
       </c>
       <c t="n" r="D227">
-        <v>174000.0</v>
+        <v>94500.0</v>
       </c>
       <c t="s" r="E227">
-        <v>359</v>
+        <v>345</v>
       </c>
       <c t="s" r="F227">
         <v>350</v>
@@ -6177,16 +6177,16 @@
     </row>
     <row spans="1:7" r="228">
       <c t="s" r="A228">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c t="s" r="B228">
-        <v>364</v>
+        <v>246</v>
       </c>
       <c t="s" r="C228">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c t="n" r="D228">
-        <v>94500.0</v>
+        <v>447000.0</v>
       </c>
       <c t="s" r="E228">
         <v>345</v>
@@ -6197,16 +6197,16 @@
     </row>
     <row spans="1:7" r="229">
       <c t="s" r="A229">
-        <v>349</v>
+        <v>124</v>
       </c>
       <c t="s" r="B229">
-        <v>246</v>
+        <v>224</v>
       </c>
       <c t="s" r="C229">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c t="n" r="D229">
-        <v>447000.0</v>
+        <v>30000.0</v>
       </c>
       <c t="s" r="E229">
         <v>345</v>
@@ -6217,13 +6217,13 @@
     </row>
     <row spans="1:7" r="230">
       <c t="s" r="A230">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c t="s" r="B230">
         <v>224</v>
       </c>
       <c t="s" r="C230">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c t="n" r="D230">
         <v>30000.0</v>
@@ -6237,13 +6237,13 @@
     </row>
     <row spans="1:7" r="231">
       <c t="s" r="A231">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c t="s" r="B231">
         <v>224</v>
       </c>
       <c t="s" r="C231">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c t="n" r="D231">
         <v>30000.0</v>
@@ -6257,41 +6257,21 @@
     </row>
     <row spans="1:7" r="232">
       <c t="s" r="A232">
-        <v>126</v>
+        <v>286</v>
       </c>
       <c t="s" r="B232">
-        <v>224</v>
+        <v>248</v>
       </c>
       <c t="s" r="C232">
-        <v>99</v>
+        <v>74</v>
       </c>
       <c t="n" r="D232">
-        <v>30000.0</v>
+        <v>98000.0</v>
       </c>
       <c t="s" r="E232">
-        <v>345</v>
+        <v>285</v>
       </c>
       <c t="s" r="F232">
-        <v>350</v>
-      </c>
-    </row>
-    <row spans="1:7" r="233">
-      <c t="s" r="A233">
-        <v>286</v>
-      </c>
-      <c t="s" r="B233">
-        <v>248</v>
-      </c>
-      <c t="s" r="C233">
-        <v>74</v>
-      </c>
-      <c t="n" r="D233">
-        <v>98000.0</v>
-      </c>
-      <c t="s" r="E233">
-        <v>285</v>
-      </c>
-      <c t="s" r="F233">
         <v>350</v>
       </c>
     </row>

</xml_diff>